<commit_message>
made some bless effect #97
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Bless.xlsx
+++ b/ConfigData/Xlsx/Bless.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="85">
   <si>
     <t>序列</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -76,34 +76,281 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>快速</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>缓慢</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次移动消耗食物-1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次移动消耗食物+1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>slow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>强度等级</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>fast</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>快速</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>缓慢</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次移动消耗食物-1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次移动消耗食物+1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>slow</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次移动消耗食物-2</t>
-  </si>
-  <si>
-    <t>快速2</t>
+    <t>金币奖励系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>食物奖励系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>生命奖励系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>精神奖励系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>经验奖励系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>金币惩罚系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>食物惩罚系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>生命惩罚系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>精神惩罚系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardFoodMulti</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardHealthMulti</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardMentalMulti</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardExpMulti</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PunishGoldMulti</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PunishFoodMulti</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PunishHealthMulti</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PunishMentalMulti</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardGoldMulti</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>money1</t>
+  </si>
+  <si>
+    <t>money2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>升值</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>负债</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务获得金钱时可以获得额外一份</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务消耗金钱时需要支付额外一份</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>food1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>food2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>恶鬼</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务获得食物时可以获得额外一份</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务消耗食物时需要支付额外一份</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>素食</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>厚甲</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务回复生命时可以获得额外一次回复</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务受到生命惩罚时会额外多触发一次</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>health1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>health2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>血咒</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>庇护</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mental1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mental2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>噩梦</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务回复精神时可以获得额外一次回复</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务受到精神惩罚时会额外多触发一次</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>发明</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>expsub</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>expadd</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>困惑</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务获得经验时可以获得额外一次</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>无法通过任务获得经验</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>roll点成功加金币</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>roll点失败扣血</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RollWinAddGold</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RollFailSubHealth</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>rollfail</t>
+  </si>
+  <si>
+    <t>rollwin</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>赌神</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>巫毒</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务中roll点失败，会受到一次生命惩罚</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务中roll点成功，会获得一次金钱奖励</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -291,7 +538,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -481,6 +728,42 @@
       <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -762,7 +1045,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -788,6 +1071,33 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -836,7 +1146,34 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1071,14 +1408,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:F6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6" headerRowCellStyle="百分比">
-  <autoFilter ref="A3:F6"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Id" dataDxfId="5"/>
-    <tableColumn id="14" name="Type" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:R17" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7" headerRowCellStyle="百分比">
+  <autoFilter ref="A3:R17"/>
+  <tableColumns count="18">
+    <tableColumn id="1" name="Id" dataDxfId="6"/>
+    <tableColumn id="14" name="Type" dataDxfId="5"/>
+    <tableColumn id="5" name="Level" dataDxfId="0"/>
     <tableColumn id="2" name="Name" dataDxfId="4"/>
     <tableColumn id="3" name="Descript" dataDxfId="3"/>
     <tableColumn id="4" name="MoveFoodChange" dataDxfId="2"/>
+    <tableColumn id="8" name="RewardGoldMulti"/>
+    <tableColumn id="7" name="RewardFoodMulti"/>
+    <tableColumn id="6" name="RewardHealthMulti"/>
+    <tableColumn id="10" name="RewardMentalMulti"/>
+    <tableColumn id="11" name="RewardExpMulti"/>
+    <tableColumn id="12" name="PunishGoldMulti"/>
+    <tableColumn id="16" name="PunishFoodMulti"/>
+    <tableColumn id="15" name="PunishHealthMulti"/>
+    <tableColumn id="13" name="PunishMentalMulti"/>
+    <tableColumn id="17" name="RollWinAddGold"/>
+    <tableColumn id="18" name="RollFailSubHealth"/>
     <tableColumn id="9" name="Icon" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1372,21 +1721,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="4" max="4" width="22.875" customWidth="1"/>
-    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.125" customWidth="1"/>
+    <col min="5" max="5" width="34.375" customWidth="1"/>
+    <col min="6" max="6" width="4.5" customWidth="1"/>
+    <col min="7" max="17" width="3.875" customWidth="1"/>
+    <col min="21" max="21" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1394,19 +1745,55 @@
         <v>3</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q1" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1414,19 +1801,55 @@
         <v>5</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="R2" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -1434,76 +1857,374 @@
         <v>10</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q3" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="R3" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>16000001</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
+      <c r="C4" s="1">
+        <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4">
         <v>-1</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
+      <c r="R4" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>16000002</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
+      <c r="C5" s="1">
+        <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>15</v>
+        <v>45</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
+        <v>16000003</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A7" s="1">
+        <v>16000004</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A8" s="1">
+        <v>16000005</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A9" s="1">
+        <v>16000006</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A10" s="1">
+        <v>16000007</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A11" s="1">
         <v>16010001</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B11" s="1">
         <v>2</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="R11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>20</v>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A12" s="1">
+        <v>16010002</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A13" s="1">
+        <v>16010003</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A14" s="1">
+        <v>16010004</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A15" s="1">
+        <v>16010005</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A16" s="1">
+        <v>16010006</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K16">
+        <v>-1</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A17" s="1">
+        <v>16010007</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add 2 fight related bless #97
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Bless.xlsx
+++ b/ConfigData/Xlsx/Bless.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="102">
   <si>
     <t>序列</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -351,6 +351,74 @@
   </si>
   <si>
     <t>每次任务中roll点成功，会获得一次金钱奖励</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗等级调整</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FightLevelChange</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗获胜加血</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗失败扣血</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FightWinAddHealth</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FightFailSubHealth</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗失败扣精神</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FightFailSubMental</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗获胜加经验</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FightWinAddExp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fightwin</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fightfail</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>吸血鬼</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次战斗获胜，会获得一次生命回复奖励</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>胆小鬼</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次战斗失败，会获得一次生命惩罚</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1408,9 +1476,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:R17" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7" headerRowCellStyle="百分比">
-  <autoFilter ref="A3:R17"/>
-  <tableColumns count="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:W19" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7" headerRowCellStyle="百分比">
+  <autoFilter ref="A3:W19"/>
+  <tableColumns count="23">
     <tableColumn id="1" name="Id" dataDxfId="6"/>
     <tableColumn id="14" name="Type" dataDxfId="5"/>
     <tableColumn id="5" name="Level" dataDxfId="0"/>
@@ -1428,6 +1496,11 @@
     <tableColumn id="13" name="PunishMentalMulti"/>
     <tableColumn id="17" name="RollWinAddGold"/>
     <tableColumn id="18" name="RollFailSubHealth"/>
+    <tableColumn id="19" name="FightLevelChange"/>
+    <tableColumn id="21" name="FightWinAddHealth"/>
+    <tableColumn id="24" name="FightWinAddExp"/>
+    <tableColumn id="22" name="FightFailSubHealth"/>
+    <tableColumn id="23" name="FightFailSubMental"/>
     <tableColumn id="9" name="Icon" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1721,10 +1794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R17"/>
+  <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1733,11 +1806,11 @@
     <col min="2" max="3" width="5.125" customWidth="1"/>
     <col min="5" max="5" width="34.375" customWidth="1"/>
     <col min="6" max="6" width="4.5" customWidth="1"/>
-    <col min="7" max="17" width="3.875" customWidth="1"/>
-    <col min="21" max="21" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="22" width="3.875" customWidth="1"/>
+    <col min="26" max="26" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1789,11 +1862,26 @@
       <c r="Q1" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="S1" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="T1" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="U1" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="V1" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="W1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1845,11 +1933,26 @@
       <c r="Q2" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="S2" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="T2" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="U2" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="V2" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="W2" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -1901,11 +2004,26 @@
       <c r="Q3" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="R3" s="8" t="s">
+      <c r="R3" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="S3" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="T3" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="U3" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="V3" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="W3" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>16000001</v>
       </c>
@@ -1924,11 +2042,11 @@
       <c r="F4">
         <v>-1</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>16000002</v>
       </c>
@@ -1947,11 +2065,11 @@
       <c r="G5">
         <v>1</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="W5" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>16000003</v>
       </c>
@@ -1970,11 +2088,11 @@
       <c r="H6">
         <v>1</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="W6" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>16000004</v>
       </c>
@@ -1993,11 +2111,11 @@
       <c r="I7">
         <v>1</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="W7" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>16000005</v>
       </c>
@@ -2016,11 +2134,11 @@
       <c r="J8">
         <v>1</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="W8" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>16000006</v>
       </c>
@@ -2039,11 +2157,11 @@
       <c r="K9">
         <v>1</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="W9" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>16000007</v>
       </c>
@@ -2062,36 +2180,36 @@
       <c r="Q10">
         <v>1</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="W10" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
+        <v>16000008</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A12" s="1">
         <v>16010001</v>
-      </c>
-      <c r="B11" s="1">
-        <v>2</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A12" s="1">
-        <v>16010002</v>
       </c>
       <c r="B12" s="1">
         <v>2</v>
@@ -2100,21 +2218,21 @@
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>44</v>
+        <v>18</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
-        <v>16010003</v>
+        <v>16010002</v>
       </c>
       <c r="B13" s="1">
         <v>2</v>
@@ -2123,21 +2241,21 @@
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
-        <v>16010004</v>
+        <v>16010003</v>
       </c>
       <c r="B14" s="1">
         <v>2</v>
@@ -2146,21 +2264,21 @@
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="N14">
-        <v>1</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
-        <v>16010005</v>
+        <v>16010004</v>
       </c>
       <c r="B15" s="1">
         <v>2</v>
@@ -2169,21 +2287,21 @@
         <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O15">
-        <v>1</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
-        <v>16010006</v>
+        <v>16010005</v>
       </c>
       <c r="B16" s="1">
         <v>2</v>
@@ -2192,21 +2310,21 @@
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K16">
-        <v>-1</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
-        <v>16010007</v>
+        <v>16010006</v>
       </c>
       <c r="B17" s="1">
         <v>2</v>
@@ -2215,16 +2333,62 @@
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K17">
+        <v>-1</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A18" s="1">
+        <v>16010007</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="P17">
-        <v>1</v>
-      </c>
-      <c r="R17" s="1" t="s">
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="W18" s="1" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A19" s="1">
+        <v>16010008</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="U19">
+        <v>1</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish some high level bless #97
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Bless.xlsx
+++ b/ConfigData/Xlsx/Bless.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="114">
   <si>
     <t>序列</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -203,229 +203,276 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>每次任务消耗金钱时需要支付额外一份</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>food1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>food2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>恶鬼</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务获得食物时可以获得额外一份</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务消耗食物时需要支付额外一份</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>素食</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>厚甲</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务回复生命时可以获得额外一次回复</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务受到生命惩罚时会额外多触发一次</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>health1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>health2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>血咒</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>庇护</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mental1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mental2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>噩梦</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务回复精神时可以获得额外一次回复</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务受到精神惩罚时会额外多触发一次</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>发明</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>expsub</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>expadd</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>困惑</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务获得经验时可以获得额外一次</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>无法通过任务获得经验</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>roll点成功加金币</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>roll点失败扣血</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RollWinAddGold</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RollFailSubHealth</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>rollfail</t>
+  </si>
+  <si>
+    <t>rollwin</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>赌神</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>巫毒</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务中roll点失败，会受到一次生命惩罚</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务中roll点成功，会获得一次金钱奖励</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗等级调整</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FightLevelChange</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗获胜加血</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗失败扣血</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FightWinAddHealth</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FightFailSubHealth</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗失败扣精神</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FightFailSubMental</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗获胜加经验</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FightWinAddExp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fightwin</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fightfail</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>吸血鬼</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次战斗获胜，会获得一次生命回复奖励</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>胆小鬼</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次战斗失败，会获得一次生命惩罚</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>战神</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次战斗获胜，会获得一次生命回复奖励，并获得额外的经验值</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fightwin2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>屈从</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次战斗失败，会获得一次生命惩罚和精神惩罚</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fightfail2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>questwin</t>
+  </si>
+  <si>
+    <t>questfail</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>王权</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>遗弃</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务成功会获得额外生命/精神/金钱/食物奖励</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务失败会获得受到生命/精神/金钱/食物惩罚</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>每次任务获得金钱时可以获得额外一份</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次任务消耗金钱时需要支付额外一份</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>food1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>food2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>恶鬼</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次任务获得食物时可以获得额外一份</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次任务消耗食物时需要支付额外一份</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>素食</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>厚甲</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次任务回复生命时可以获得额外一次回复</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次任务受到生命惩罚时会额外多触发一次</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>health1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>health2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>血咒</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>庇护</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>mental1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>mental2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>噩梦</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次任务回复精神时可以获得额外一次回复</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次任务受到精神惩罚时会额外多触发一次</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>发明</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>expsub</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>expadd</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>困惑</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次任务获得经验时可以获得额外一次</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>无法通过任务获得经验</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>roll点成功加金币</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>roll点失败扣血</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RollWinAddGold</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RollFailSubHealth</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>rollfail</t>
-  </si>
-  <si>
-    <t>rollwin</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>赌神</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>巫毒</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次任务中roll点失败，会受到一次生命惩罚</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次任务中roll点成功，会获得一次金钱奖励</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>战斗等级调整</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>FightLevelChange</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>战斗获胜加血</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>战斗失败扣血</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>FightWinAddHealth</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>FightFailSubHealth</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>战斗失败扣精神</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>FightFailSubMental</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>战斗获胜加经验</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>FightWinAddExp</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>fightwin</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>fightfail</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>吸血鬼</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次战斗获胜，会获得一次生命回复奖励</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>胆小鬼</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次战斗失败，会获得一次生命惩罚</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1476,15 +1523,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:W19" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7" headerRowCellStyle="百分比">
-  <autoFilter ref="A3:W19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:W23" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7" headerRowCellStyle="百分比">
+  <autoFilter ref="A3:W23"/>
   <tableColumns count="23">
     <tableColumn id="1" name="Id" dataDxfId="6"/>
     <tableColumn id="14" name="Type" dataDxfId="5"/>
-    <tableColumn id="5" name="Level" dataDxfId="0"/>
-    <tableColumn id="2" name="Name" dataDxfId="4"/>
-    <tableColumn id="3" name="Descript" dataDxfId="3"/>
-    <tableColumn id="4" name="MoveFoodChange" dataDxfId="2"/>
+    <tableColumn id="5" name="Level" dataDxfId="4"/>
+    <tableColumn id="2" name="Name" dataDxfId="3"/>
+    <tableColumn id="3" name="Descript" dataDxfId="2"/>
+    <tableColumn id="4" name="MoveFoodChange" dataDxfId="1"/>
     <tableColumn id="8" name="RewardGoldMulti"/>
     <tableColumn id="7" name="RewardFoodMulti"/>
     <tableColumn id="6" name="RewardHealthMulti"/>
@@ -1501,14 +1548,14 @@
     <tableColumn id="24" name="FightWinAddExp"/>
     <tableColumn id="22" name="FightFailSubHealth"/>
     <tableColumn id="23" name="FightFailSubMental"/>
-    <tableColumn id="9" name="Icon" dataDxfId="1"/>
+    <tableColumn id="9" name="Icon" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1583,6 +1630,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1618,6 +1682,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1794,10 +1875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W19"/>
+  <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1857,25 +1938,25 @@
         <v>33</v>
       </c>
       <c r="P1" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q1" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R1" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S1" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="T1" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="U1" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="U1" s="15" t="s">
-        <v>89</v>
-      </c>
       <c r="V1" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="W1" s="4" t="s">
         <v>4</v>
@@ -1928,25 +2009,25 @@
         <v>29</v>
       </c>
       <c r="P2" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q2" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="Q2" s="16" t="s">
-        <v>75</v>
-      </c>
       <c r="R2" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S2" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="T2" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="U2" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V2" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="W2" s="7" t="s">
         <v>6</v>
@@ -1999,25 +2080,25 @@
         <v>41</v>
       </c>
       <c r="P3" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q3" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="Q3" s="17" t="s">
-        <v>78</v>
-      </c>
       <c r="R3" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S3" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="T3" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="U3" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="T3" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="U3" s="17" t="s">
-        <v>91</v>
-      </c>
       <c r="V3" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="W3" s="8" t="s">
         <v>11</v>
@@ -2060,7 +2141,7 @@
         <v>45</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>47</v>
+        <v>113</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -2080,16 +2161,16 @@
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.15">
@@ -2103,16 +2184,16 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="I7">
         <v>1</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.15">
@@ -2126,16 +2207,16 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="W8" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.15">
@@ -2149,16 +2230,16 @@
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K9">
         <v>1</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.15">
@@ -2172,16 +2253,16 @@
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q10">
         <v>1</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.15">
@@ -2195,67 +2276,79 @@
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="S11">
         <v>1</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
-        <v>16010001</v>
+        <v>16001001</v>
       </c>
       <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
         <v>2</v>
       </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12">
+        <v>102</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="T12">
         <v>1</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>19</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
-        <v>16010002</v>
+        <v>16002001</v>
       </c>
       <c r="B13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>46</v>
+        <v>109</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L13">
+        <v>111</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
         <v>1</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>44</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
-        <v>16010003</v>
+        <v>16010001</v>
       </c>
       <c r="B14" s="1">
         <v>2</v>
@@ -2264,21 +2357,21 @@
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="M14">
+        <v>18</v>
+      </c>
+      <c r="F14">
         <v>1</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
-        <v>16010004</v>
+        <v>16010002</v>
       </c>
       <c r="B15" s="1">
         <v>2</v>
@@ -2287,21 +2380,21 @@
         <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="N15">
+        <v>47</v>
+      </c>
+      <c r="L15">
         <v>1</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
-        <v>16010005</v>
+        <v>16010003</v>
       </c>
       <c r="B16" s="1">
         <v>2</v>
@@ -2310,21 +2403,21 @@
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O16">
+        <v>52</v>
+      </c>
+      <c r="M16">
         <v>1</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
-        <v>16010006</v>
+        <v>16010004</v>
       </c>
       <c r="B17" s="1">
         <v>2</v>
@@ -2333,21 +2426,21 @@
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K17">
-        <v>-1</v>
+        <v>56</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A18" s="1">
-        <v>16010007</v>
+        <v>16010005</v>
       </c>
       <c r="B18" s="1">
         <v>2</v>
@@ -2356,21 +2449,21 @@
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="P18">
+        <v>65</v>
+      </c>
+      <c r="O18">
         <v>1</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A19" s="1">
-        <v>16010008</v>
+        <v>16010006</v>
       </c>
       <c r="B19" s="1">
         <v>2</v>
@@ -2379,16 +2472,120 @@
         <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K19">
+        <v>-1</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A20" s="1">
+        <v>16010007</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="W20" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A21" s="1">
+        <v>16010008</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="U19">
-        <v>1</v>
-      </c>
-      <c r="W19" s="1" t="s">
-        <v>97</v>
+      <c r="U21">
+        <v>1</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A22" s="1">
+        <v>16011001</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="U22">
+        <v>1</v>
+      </c>
+      <c r="V22">
+        <v>1</v>
+      </c>
+      <c r="W22" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A23" s="1">
+        <v>16012001</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1">
+        <v>3</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="W23" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use bless to implement long walk effect
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Bless.xlsx
+++ b/ConfigData/Xlsx/Bless.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="124">
   <si>
     <t>序列</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -466,6 +466,45 @@
   </si>
   <si>
     <t>每次任务获得金钱时可以获得额外一份</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MoveDistance</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>移动距离加长</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>持续回合数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Round</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>longwalk1</t>
+  </si>
+  <si>
+    <t>运输</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>在地图移动时，每次可以多走一步</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>longwalk2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>在地图移动时，不受移动步长限制</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>飞翔</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -473,7 +512,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -652,8 +691,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="41">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -881,8 +928,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF577AD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB31D96"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1028,6 +1087,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1160,22 +1237,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1188,31 +1256,58 @@
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="39" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="41" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="41" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="42" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1261,7 +1356,21 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1511,6 +1620,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFB31D96"/>
+      <color rgb="FFF577AD"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1523,15 +1638,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:W23" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7" headerRowCellStyle="百分比">
-  <autoFilter ref="A3:W23"/>
-  <tableColumns count="23">
-    <tableColumn id="1" name="Id" dataDxfId="6"/>
-    <tableColumn id="14" name="Type" dataDxfId="5"/>
-    <tableColumn id="5" name="Level" dataDxfId="4"/>
-    <tableColumn id="2" name="Name" dataDxfId="3"/>
-    <tableColumn id="3" name="Descript" dataDxfId="2"/>
-    <tableColumn id="4" name="MoveFoodChange" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:Y25" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9" headerRowCellStyle="百分比">
+  <autoFilter ref="A3:Y25"/>
+  <tableColumns count="25">
+    <tableColumn id="1" name="Id" dataDxfId="8"/>
+    <tableColumn id="14" name="Type" dataDxfId="7"/>
+    <tableColumn id="5" name="Level" dataDxfId="6"/>
+    <tableColumn id="2" name="Name" dataDxfId="5"/>
+    <tableColumn id="3" name="Descript" dataDxfId="4"/>
+    <tableColumn id="25" name="Round"/>
+    <tableColumn id="4" name="MoveFoodChange" dataDxfId="3"/>
+    <tableColumn id="20" name="MoveDistance"/>
     <tableColumn id="8" name="RewardGoldMulti"/>
     <tableColumn id="7" name="RewardFoodMulti"/>
     <tableColumn id="6" name="RewardHealthMulti"/>
@@ -1548,7 +1665,7 @@
     <tableColumn id="24" name="FightWinAddExp"/>
     <tableColumn id="22" name="FightFailSubHealth"/>
     <tableColumn id="23" name="FightFailSubMental"/>
-    <tableColumn id="9" name="Icon" dataDxfId="0"/>
+    <tableColumn id="9" name="Icon" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1875,10 +1992,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W23"/>
+  <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1886,710 +2003,851 @@
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="5.125" customWidth="1"/>
     <col min="5" max="5" width="34.375" customWidth="1"/>
-    <col min="6" max="6" width="4.5" customWidth="1"/>
-    <col min="7" max="22" width="3.875" customWidth="1"/>
-    <col min="26" max="26" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.875" customWidth="1"/>
+    <col min="7" max="8" width="4.5" customWidth="1"/>
+    <col min="9" max="24" width="3.875" customWidth="1"/>
+    <col min="28" max="28" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:25" ht="66" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="J1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="K1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="L1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="M1" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="N1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="O1" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="P1" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="Q1" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="R1" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="S1" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="T1" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Y1" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="I2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="J2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="K2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="L2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="M2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="N2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="O2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="P2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="16" t="s">
+      <c r="Q2" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="S2" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="R2" s="16" t="s">
+      <c r="T2" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="U2" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="T2" s="16" t="s">
+      <c r="V2" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="U2" s="16" t="s">
+      <c r="W2" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="V2" s="16" t="s">
+      <c r="X2" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="Y2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="H3" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="J3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="K3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="L3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="M3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="N3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="O3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="N3" s="14" t="s">
+      <c r="P3" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O3" s="14" t="s">
+      <c r="Q3" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="P3" s="17" t="s">
+      <c r="R3" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="Q3" s="17" t="s">
+      <c r="S3" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="R3" s="17" t="s">
+      <c r="T3" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="S3" s="17" t="s">
+      <c r="U3" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="T3" s="17" t="s">
+      <c r="V3" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="U3" s="17" t="s">
+      <c r="W3" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="V3" s="17" t="s">
+      <c r="X3" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="W3" s="8" t="s">
+      <c r="Y3" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>16000001</v>
       </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>17</v>
       </c>
       <c r="F4">
+        <v>30</v>
+      </c>
+      <c r="G4">
         <v>-1</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="Y4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>16000002</v>
       </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>113</v>
       </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="W5" s="1" t="s">
+      <c r="F5">
+        <v>30</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="Y5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>16000003</v>
       </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>51</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="W6" s="1" t="s">
+      <c r="F6">
+        <v>30</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="Y6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>16000004</v>
       </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>55</v>
       </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="W7" s="1" t="s">
+      <c r="F7">
+        <v>30</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="Y7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>16000005</v>
       </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>64</v>
       </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="W8" s="1" t="s">
+      <c r="F8">
+        <v>30</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="Y8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>16000006</v>
       </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>70</v>
       </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="W9" s="1" t="s">
+      <c r="F9">
+        <v>30</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="Y9" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>16000007</v>
       </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
         <v>80</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>83</v>
       </c>
-      <c r="Q10">
-        <v>1</v>
-      </c>
-      <c r="W10" s="1" t="s">
+      <c r="F10">
+        <v>30</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="Y10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>16000008</v>
       </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
         <v>97</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>98</v>
       </c>
-      <c r="S11">
-        <v>1</v>
-      </c>
-      <c r="W11" s="1" t="s">
+      <c r="F11">
+        <v>30</v>
+      </c>
+      <c r="U11">
+        <v>1</v>
+      </c>
+      <c r="Y11" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
+        <v>16000009</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>119</v>
+      </c>
+      <c r="E12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="23" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A13" s="1">
         <v>16001001</v>
       </c>
-      <c r="B12" s="1">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
         <v>2</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D13" t="s">
         <v>101</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E13" t="s">
         <v>102</v>
       </c>
-      <c r="S12">
-        <v>1</v>
-      </c>
-      <c r="T12">
-        <v>1</v>
-      </c>
-      <c r="W12" s="1" t="s">
+      <c r="F13">
+        <v>30</v>
+      </c>
+      <c r="U13">
+        <v>1</v>
+      </c>
+      <c r="V13">
+        <v>1</v>
+      </c>
+      <c r="Y13" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A13" s="1">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A14" s="1">
         <v>16002001</v>
       </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
         <v>3</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D14" t="s">
         <v>109</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E14" t="s">
         <v>111</v>
       </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="W13" s="1" t="s">
+      <c r="F14">
+        <v>30</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="Y14" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A14" s="1">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A15" s="1">
+        <v>16002002</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>123</v>
+      </c>
+      <c r="E15" t="s">
+        <v>122</v>
+      </c>
+      <c r="F15">
+        <v>10</v>
+      </c>
+      <c r="H15">
+        <v>98</v>
+      </c>
+      <c r="Y15" s="23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A16" s="1">
         <v>16010001</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B16">
         <v>2</v>
       </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E16" t="s">
         <v>18</v>
       </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="W14" s="1" t="s">
+      <c r="F16">
+        <v>30</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="Y16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A15" s="1">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A17" s="1">
         <v>16010002</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B17">
         <v>2</v>
       </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E17" t="s">
         <v>47</v>
       </c>
-      <c r="L15">
-        <v>1</v>
-      </c>
-      <c r="W15" s="1" t="s">
+      <c r="F17">
+        <v>30</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="Y17" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A16" s="1">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A18" s="1">
         <v>16010003</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B18">
         <v>2</v>
       </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E18" t="s">
         <v>52</v>
       </c>
-      <c r="M16">
-        <v>1</v>
-      </c>
-      <c r="W16" s="1" t="s">
+      <c r="F18">
+        <v>30</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="Y18" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A17" s="1">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A19" s="1">
         <v>16010004</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B19">
         <v>2</v>
       </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E19" t="s">
         <v>56</v>
       </c>
-      <c r="N17">
-        <v>1</v>
-      </c>
-      <c r="W17" s="1" t="s">
+      <c r="F19">
+        <v>30</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Y19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A18" s="1">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A20" s="1">
         <v>16010005</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B20">
         <v>2</v>
       </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1" t="s">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E20" t="s">
         <v>65</v>
       </c>
-      <c r="O18">
-        <v>1</v>
-      </c>
-      <c r="W18" s="1" t="s">
+      <c r="F20">
+        <v>30</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="Y20" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A19" s="1">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A21" s="1">
         <v>16010006</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B21">
         <v>2</v>
       </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E21" t="s">
         <v>71</v>
       </c>
-      <c r="K19">
+      <c r="F21">
+        <v>30</v>
+      </c>
+      <c r="M21">
         <v>-1</v>
       </c>
-      <c r="W19" s="1" t="s">
+      <c r="Y21" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A20" s="1">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A22" s="1">
         <v>16010007</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B22">
         <v>2</v>
       </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E22" t="s">
         <v>82</v>
       </c>
-      <c r="P20">
-        <v>1</v>
-      </c>
-      <c r="W20" s="1" t="s">
+      <c r="F22">
+        <v>30</v>
+      </c>
+      <c r="R22">
+        <v>1</v>
+      </c>
+      <c r="Y22" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A21" s="1">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A23" s="1">
         <v>16010008</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B23">
         <v>2</v>
       </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1" t="s">
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
         <v>99</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E23" t="s">
         <v>100</v>
       </c>
-      <c r="U21">
-        <v>1</v>
-      </c>
-      <c r="W21" s="1" t="s">
+      <c r="F23">
+        <v>30</v>
+      </c>
+      <c r="W23">
+        <v>1</v>
+      </c>
+      <c r="Y23" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A22" s="1">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A24" s="1">
         <v>16011001</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B24">
         <v>2</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C24">
         <v>2</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D24" t="s">
         <v>104</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E24" t="s">
         <v>105</v>
       </c>
-      <c r="U22">
-        <v>1</v>
-      </c>
-      <c r="V22">
-        <v>1</v>
-      </c>
-      <c r="W22" s="1" t="s">
+      <c r="F24">
+        <v>30</v>
+      </c>
+      <c r="W24">
+        <v>1</v>
+      </c>
+      <c r="X24">
+        <v>1</v>
+      </c>
+      <c r="Y24" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A23" s="1">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A25" s="1">
         <v>16012001</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B25">
         <v>2</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C25">
         <v>3</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D25" t="s">
         <v>110</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E25" t="s">
         <v>112</v>
       </c>
-      <c r="L23">
-        <v>1</v>
-      </c>
-      <c r="M23">
-        <v>1</v>
-      </c>
-      <c r="N23">
-        <v>1</v>
-      </c>
-      <c r="O23">
-        <v>1</v>
-      </c>
-      <c r="W23" s="1" t="s">
+      <c r="F25">
+        <v>30</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
+      <c r="Y25" t="s">
         <v>108</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
+  <conditionalFormatting sqref="B4:Y14 B16:Y25">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(B4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:Y15">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(B15))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
distinguish the bless type by enum. add a new type "quest"
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Bless.xlsx
+++ b/ConfigData/Xlsx/Bless.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="126">
   <si>
     <t>序列</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -505,6 +505,14 @@
   </si>
   <si>
     <t>飞翔</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ropeway</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>滑道</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -700,7 +708,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="43">
+  <fills count="46">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -938,6 +946,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB31D96"/>
         <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1237,11 +1263,8 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
@@ -1308,6 +1331,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="45" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1356,7 +1388,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill>
@@ -1618,6 +1650,20 @@
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1638,8 +1684,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:Y25" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9" headerRowCellStyle="百分比">
-  <autoFilter ref="A3:Y25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:Y26" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9" headerRowCellStyle="百分比">
+  <autoFilter ref="A3:Y26"/>
   <tableColumns count="25">
     <tableColumn id="1" name="Id" dataDxfId="8"/>
     <tableColumn id="14" name="Type" dataDxfId="7"/>
@@ -1992,10 +2038,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y25"/>
+  <dimension ref="A1:Y26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2010,238 +2056,238 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="66" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="10" t="s">
+      <c r="D1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="Q1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="R1" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="S1" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="T1" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="U1" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="V1" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="W1" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="X1" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="Y1" s="11" t="s">
+      <c r="Y1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="18" t="s">
+      <c r="N2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="18" t="s">
+      <c r="O2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="18" t="s">
+      <c r="P2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="18" t="s">
+      <c r="Q2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="R2" s="19" t="s">
+      <c r="R2" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="S2" s="19" t="s">
+      <c r="S2" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="T2" s="19" t="s">
+      <c r="T2" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="U2" s="19" t="s">
+      <c r="U2" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="V2" s="19" t="s">
+      <c r="V2" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="W2" s="19" t="s">
+      <c r="W2" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="X2" s="19" t="s">
+      <c r="X2" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Y2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="P3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="Q3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="R3" s="8" t="s">
+      <c r="R3" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="S3" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="T3" s="8" t="s">
+      <c r="T3" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="U3" s="8" t="s">
+      <c r="U3" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="V3" s="8" t="s">
+      <c r="V3" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="W3" s="8" t="s">
+      <c r="W3" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="X3" s="8" t="s">
+      <c r="X3" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="Y3" s="5" t="s">
+      <c r="Y3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A4" s="1">
+      <c r="A4" s="23">
         <v>16000001</v>
       </c>
       <c r="B4">
@@ -2257,7 +2303,7 @@
         <v>17</v>
       </c>
       <c r="F4">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G4">
         <v>-1</v>
@@ -2267,7 +2313,7 @@
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A5" s="1">
+      <c r="A5" s="23">
         <v>16000002</v>
       </c>
       <c r="B5">
@@ -2283,7 +2329,7 @@
         <v>113</v>
       </c>
       <c r="F5">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -2293,7 +2339,7 @@
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A6" s="1">
+      <c r="A6" s="23">
         <v>16000003</v>
       </c>
       <c r="B6">
@@ -2309,7 +2355,7 @@
         <v>51</v>
       </c>
       <c r="F6">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -2319,7 +2365,7 @@
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A7" s="1">
+      <c r="A7" s="23">
         <v>16000004</v>
       </c>
       <c r="B7">
@@ -2335,7 +2381,7 @@
         <v>55</v>
       </c>
       <c r="F7">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -2345,7 +2391,7 @@
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A8" s="1">
+      <c r="A8" s="23">
         <v>16000005</v>
       </c>
       <c r="B8">
@@ -2361,7 +2407,7 @@
         <v>64</v>
       </c>
       <c r="F8">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="L8">
         <v>1</v>
@@ -2371,7 +2417,7 @@
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A9" s="1">
+      <c r="A9" s="23">
         <v>16000006</v>
       </c>
       <c r="B9">
@@ -2387,7 +2433,7 @@
         <v>70</v>
       </c>
       <c r="F9">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="M9">
         <v>1</v>
@@ -2397,7 +2443,7 @@
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A10" s="1">
+      <c r="A10" s="23">
         <v>16000007</v>
       </c>
       <c r="B10">
@@ -2413,7 +2459,7 @@
         <v>83</v>
       </c>
       <c r="F10">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="S10">
         <v>1</v>
@@ -2423,7 +2469,7 @@
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A11" s="1">
+      <c r="A11" s="23">
         <v>16000008</v>
       </c>
       <c r="B11">
@@ -2439,7 +2485,7 @@
         <v>98</v>
       </c>
       <c r="F11">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="U11">
         <v>1</v>
@@ -2449,7 +2495,7 @@
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A12" s="1">
+      <c r="A12" s="23">
         <v>16000009</v>
       </c>
       <c r="B12">
@@ -2470,12 +2516,12 @@
       <c r="H12">
         <v>1</v>
       </c>
-      <c r="Y12" s="23" t="s">
+      <c r="Y12" s="22" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A13" s="1">
+      <c r="A13" s="23">
         <v>16001001</v>
       </c>
       <c r="B13">
@@ -2491,7 +2537,7 @@
         <v>102</v>
       </c>
       <c r="F13">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="U13">
         <v>1</v>
@@ -2504,7 +2550,7 @@
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A14" s="1">
+      <c r="A14" s="23">
         <v>16002001</v>
       </c>
       <c r="B14">
@@ -2520,7 +2566,7 @@
         <v>111</v>
       </c>
       <c r="F14">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -2539,7 +2585,7 @@
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A15" s="1">
+      <c r="A15" s="23">
         <v>16002002</v>
       </c>
       <c r="B15">
@@ -2560,12 +2606,12 @@
       <c r="H15">
         <v>98</v>
       </c>
-      <c r="Y15" s="23" t="s">
+      <c r="Y15" s="22" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A16" s="1">
+      <c r="A16" s="24">
         <v>16010001</v>
       </c>
       <c r="B16">
@@ -2581,7 +2627,7 @@
         <v>18</v>
       </c>
       <c r="F16">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -2591,7 +2637,7 @@
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A17" s="1">
+      <c r="A17" s="24">
         <v>16010002</v>
       </c>
       <c r="B17">
@@ -2607,7 +2653,7 @@
         <v>47</v>
       </c>
       <c r="F17">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="N17">
         <v>1</v>
@@ -2617,7 +2663,7 @@
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A18" s="1">
+      <c r="A18" s="24">
         <v>16010003</v>
       </c>
       <c r="B18">
@@ -2633,7 +2679,7 @@
         <v>52</v>
       </c>
       <c r="F18">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="O18">
         <v>1</v>
@@ -2643,7 +2689,7 @@
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A19" s="1">
+      <c r="A19" s="24">
         <v>16010004</v>
       </c>
       <c r="B19">
@@ -2659,7 +2705,7 @@
         <v>56</v>
       </c>
       <c r="F19">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="P19">
         <v>1</v>
@@ -2669,7 +2715,7 @@
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A20" s="1">
+      <c r="A20" s="24">
         <v>16010005</v>
       </c>
       <c r="B20">
@@ -2685,7 +2731,7 @@
         <v>65</v>
       </c>
       <c r="F20">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="Q20">
         <v>1</v>
@@ -2695,7 +2741,7 @@
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A21" s="1">
+      <c r="A21" s="24">
         <v>16010006</v>
       </c>
       <c r="B21">
@@ -2711,7 +2757,7 @@
         <v>71</v>
       </c>
       <c r="F21">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="M21">
         <v>-1</v>
@@ -2721,7 +2767,7 @@
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A22" s="1">
+      <c r="A22" s="24">
         <v>16010007</v>
       </c>
       <c r="B22">
@@ -2737,7 +2783,7 @@
         <v>82</v>
       </c>
       <c r="F22">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="R22">
         <v>1</v>
@@ -2747,7 +2793,7 @@
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A23" s="1">
+      <c r="A23" s="24">
         <v>16010008</v>
       </c>
       <c r="B23">
@@ -2763,7 +2809,7 @@
         <v>100</v>
       </c>
       <c r="F23">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="W23">
         <v>1</v>
@@ -2773,7 +2819,7 @@
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A24" s="1">
+      <c r="A24" s="24">
         <v>16011001</v>
       </c>
       <c r="B24">
@@ -2789,7 +2835,7 @@
         <v>105</v>
       </c>
       <c r="F24">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="W24">
         <v>1</v>
@@ -2802,7 +2848,7 @@
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A25" s="1">
+      <c r="A25" s="24">
         <v>16012001</v>
       </c>
       <c r="B25">
@@ -2818,7 +2864,7 @@
         <v>112</v>
       </c>
       <c r="F25">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="N25">
         <v>1</v>
@@ -2834,18 +2880,55 @@
       </c>
       <c r="Y25" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A26" s="25">
+        <v>16020001</v>
+      </c>
+      <c r="B26" s="22">
+        <v>3</v>
+      </c>
+      <c r="C26" s="22">
+        <v>1</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="E26" t="s">
+        <v>122</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26" s="22"/>
+      <c r="H26">
+        <v>98</v>
+      </c>
+      <c r="Y26" s="22" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B4:Y14 B16:Y25">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+  <conditionalFormatting sqref="B4:Y4 B16:E25 G16:Y25 B5:E14 G5:Y14 F5:F25">
+    <cfRule type="containsBlanks" dxfId="13" priority="4">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15:Y15">
+  <conditionalFormatting sqref="B15:E15 G15:Y15">
+    <cfRule type="containsBlanks" dxfId="12" priority="3">
+      <formula>LEN(TRIM(B15))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26:D26 F26:Y26">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(B26))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B15))=0</formula>
+      <formula>LEN(TRIM(E26))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add a new bless event
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Bless.xlsx
+++ b/ConfigData/Xlsx/Bless.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="138">
   <si>
     <t>序列</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -342,14 +342,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>每次任务中roll点失败，会受到一次生命惩罚</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次任务中roll点成功，会获得一次金钱奖励</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>战斗等级调整</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -513,6 +505,62 @@
   </si>
   <si>
     <t>滑道</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次触发[失败]或[大失败]时，会受到一次生命惩罚</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次触发[成功]或[大成功]时，会获得一次金钱奖励</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>一直大失败</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RollAlwaysFailBig</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>你的所有[失败]被认定为[大失败]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>怯懦</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>一直大成功</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RollAlwaysWinBig</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>谦逊</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>你的所有[成功]被认定为[大成功]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>rollwin2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>rollfail3</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -708,7 +756,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="46">
+  <fills count="48">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -963,6 +1011,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1263,7 +1323,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1340,6 +1400,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="45" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="46" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="46" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1388,7 +1460,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -1397,11 +1469,7 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <font>
@@ -1650,23 +1718,75 @@
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
     <mruColors>
       <color rgb="FFB31D96"/>
       <color rgb="FFF577AD"/>
@@ -1684,9 +1804,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:Y26" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9" headerRowCellStyle="百分比">
-  <autoFilter ref="A3:Y26"/>
-  <tableColumns count="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AA28" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9" headerRowCellStyle="百分比">
+  <autoFilter ref="A3:AA28"/>
+  <tableColumns count="27">
     <tableColumn id="1" name="Id" dataDxfId="8"/>
     <tableColumn id="14" name="Type" dataDxfId="7"/>
     <tableColumn id="5" name="Level" dataDxfId="6"/>
@@ -1706,6 +1826,8 @@
     <tableColumn id="13" name="PunishMentalMulti"/>
     <tableColumn id="17" name="RollWinAddGold"/>
     <tableColumn id="18" name="RollFailSubHealth"/>
+    <tableColumn id="27" name="RollAlwaysWinBig"/>
+    <tableColumn id="26" name="RollAlwaysFailBig" dataDxfId="1"/>
     <tableColumn id="19" name="FightLevelChange"/>
     <tableColumn id="21" name="FightWinAddHealth"/>
     <tableColumn id="24" name="FightWinAddExp"/>
@@ -1725,7 +1847,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2038,10 +2160,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y26"/>
+  <dimension ref="A1:AA28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2051,11 +2173,13 @@
     <col min="5" max="5" width="34.375" customWidth="1"/>
     <col min="6" max="6" width="4.875" customWidth="1"/>
     <col min="7" max="8" width="4.5" customWidth="1"/>
-    <col min="9" max="24" width="3.875" customWidth="1"/>
-    <col min="28" max="28" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="19" width="3.875" customWidth="1"/>
+    <col min="20" max="21" width="4.5" customWidth="1"/>
+    <col min="22" max="26" width="3.875" customWidth="1"/>
+    <col min="30" max="30" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="66" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:27" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2072,13 +2196,13 @@
         <v>2</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G1" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>24</v>
@@ -2107,32 +2231,38 @@
       <c r="Q1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="R1" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="S1" s="14" t="s">
+      <c r="S1" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="T1" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="U1" s="14" t="s">
-        <v>87</v>
+      <c r="T1" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="U1" s="27" t="s">
+        <v>126</v>
       </c>
       <c r="V1" s="14" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="W1" s="14" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="X1" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="Y1" s="10" t="s">
+      <c r="Y1" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2184,32 +2314,38 @@
       <c r="Q2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="R2" s="18" t="s">
+      <c r="R2" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="S2" s="18" t="s">
+      <c r="S2" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="T2" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="U2" s="18" t="s">
-        <v>85</v>
+      <c r="T2" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="U2" s="28" t="s">
+        <v>127</v>
       </c>
       <c r="V2" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="W2" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="X2" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y2" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z2" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -2226,13 +2362,13 @@
         <v>9</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>42</v>
@@ -2261,32 +2397,38 @@
       <c r="Q3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="R3" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="S3" s="7" t="s">
+      <c r="S3" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="T3" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="U3" s="7" t="s">
-        <v>89</v>
+      <c r="T3" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="U3" s="29" t="s">
+        <v>128</v>
       </c>
       <c r="V3" s="7" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="W3" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="X3" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="Y3" s="4" t="s">
+      <c r="Y3" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z3" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A4" s="23">
         <v>16000001</v>
       </c>
@@ -2308,11 +2450,12 @@
       <c r="G4">
         <v>-1</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="U4" s="26"/>
+      <c r="AA4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A5" s="23">
         <v>16000002</v>
       </c>
@@ -2326,7 +2469,7 @@
         <v>45</v>
       </c>
       <c r="E5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F5">
         <v>20</v>
@@ -2334,11 +2477,12 @@
       <c r="I5">
         <v>1</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="U5" s="26"/>
+      <c r="AA5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A6" s="23">
         <v>16000003</v>
       </c>
@@ -2360,11 +2504,12 @@
       <c r="J6">
         <v>1</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="U6" s="26"/>
+      <c r="AA6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A7" s="23">
         <v>16000004</v>
       </c>
@@ -2386,11 +2531,12 @@
       <c r="K7">
         <v>1</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="U7" s="26"/>
+      <c r="AA7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A8" s="23">
         <v>16000005</v>
       </c>
@@ -2412,11 +2558,12 @@
       <c r="L8">
         <v>1</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="U8" s="26"/>
+      <c r="AA8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A9" s="23">
         <v>16000006</v>
       </c>
@@ -2438,11 +2585,12 @@
       <c r="M9">
         <v>1</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="U9" s="26"/>
+      <c r="AA9" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A10" s="23">
         <v>16000007</v>
       </c>
@@ -2456,7 +2604,7 @@
         <v>80</v>
       </c>
       <c r="E10" t="s">
-        <v>83</v>
+        <v>125</v>
       </c>
       <c r="F10">
         <v>20</v>
@@ -2464,11 +2612,12 @@
       <c r="S10">
         <v>1</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="U10" s="26"/>
+      <c r="AA10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A11" s="23">
         <v>16000008</v>
       </c>
@@ -2479,22 +2628,23 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F11">
         <v>20</v>
       </c>
-      <c r="U11">
-        <v>1</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>95</v>
+      <c r="U11" s="26"/>
+      <c r="W11">
+        <v>1</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A12" s="23">
         <v>16000009</v>
       </c>
@@ -2505,10 +2655,10 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F12">
         <v>10</v>
@@ -2516,11 +2666,12 @@
       <c r="H12">
         <v>1</v>
       </c>
-      <c r="Y12" s="22" t="s">
-        <v>118</v>
+      <c r="U12" s="26"/>
+      <c r="AA12" s="22" t="s">
+        <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A13" s="23">
         <v>16001001</v>
       </c>
@@ -2531,62 +2682,55 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F13">
         <v>20</v>
       </c>
-      <c r="U13">
-        <v>1</v>
-      </c>
-      <c r="V13">
-        <v>1</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>103</v>
+      <c r="U13" s="26"/>
+      <c r="W13">
+        <v>1</v>
+      </c>
+      <c r="X13">
+        <v>1</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A14" s="23">
+        <v>16001002</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E14" t="s">
+        <v>135</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="T14" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="U14" s="26"/>
+      <c r="AA14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="A15" s="23">
         <v>16002001</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14" t="s">
-        <v>109</v>
-      </c>
-      <c r="E14" t="s">
-        <v>111</v>
-      </c>
-      <c r="F14">
-        <v>20</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-      <c r="K14">
-        <v>1</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A15" s="23">
-        <v>16002002</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2595,50 +2739,62 @@
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="E15" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="F15">
+        <v>20</v>
+      </c>
+      <c r="G15" s="22"/>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="U15" s="26"/>
+      <c r="AA15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="A16" s="23">
+        <v>16002002</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>121</v>
+      </c>
+      <c r="E16" t="s">
+        <v>120</v>
+      </c>
+      <c r="F16">
         <v>10</v>
       </c>
-      <c r="H15">
+      <c r="H16">
         <v>98</v>
       </c>
-      <c r="Y15" s="22" t="s">
-        <v>121</v>
+      <c r="U16" s="26"/>
+      <c r="AA16" s="22" t="s">
+        <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A16" s="24">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="A17" s="24">
         <v>16010001</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16">
-        <v>20</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A17" s="24">
-        <v>16010002</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -2647,24 +2803,25 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="F17">
         <v>20</v>
       </c>
-      <c r="N17">
-        <v>1</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>44</v>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="U17" s="26"/>
+      <c r="AA17" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A18" s="24">
-        <v>16010003</v>
+        <v>16010002</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -2673,24 +2830,25 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E18" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F18">
         <v>20</v>
       </c>
-      <c r="O18">
-        <v>1</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>49</v>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="U18" s="26"/>
+      <c r="AA18" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A19" s="24">
-        <v>16010004</v>
+        <v>16010003</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -2699,24 +2857,25 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E19" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F19">
         <v>20</v>
       </c>
-      <c r="P19">
-        <v>1</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>58</v>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="U19" s="26"/>
+      <c r="AA19" t="s">
+        <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A20" s="24">
-        <v>16010005</v>
+        <v>16010004</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -2725,24 +2884,25 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E20" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="F20">
         <v>20</v>
       </c>
-      <c r="Q20">
-        <v>1</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>62</v>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="U20" s="26"/>
+      <c r="AA20" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A21" s="24">
-        <v>16010006</v>
+        <v>16010005</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -2751,24 +2911,25 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F21">
         <v>20</v>
       </c>
-      <c r="M21">
-        <v>-1</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>67</v>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="U21" s="26"/>
+      <c r="AA21" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A22" s="24">
-        <v>16010007</v>
+        <v>16010006</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -2777,24 +2938,25 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="E22" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="F22">
         <v>20</v>
       </c>
-      <c r="R22">
-        <v>1</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>78</v>
+      <c r="M22">
+        <v>-1</v>
+      </c>
+      <c r="U22" s="26"/>
+      <c r="AA22" t="s">
+        <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A23" s="24">
-        <v>16010008</v>
+        <v>16010007</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -2803,132 +2965,175 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="E23" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="F23">
         <v>20</v>
       </c>
-      <c r="W23">
-        <v>1</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>96</v>
+      <c r="R23">
+        <v>1</v>
+      </c>
+      <c r="U23" s="26"/>
+      <c r="AA23" t="s">
+        <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A24" s="24">
-        <v>16011001</v>
+        <v>16010008</v>
       </c>
       <c r="B24">
         <v>2</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E24" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="F24">
         <v>20</v>
       </c>
-      <c r="W24">
-        <v>1</v>
-      </c>
-      <c r="X24">
-        <v>1</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>106</v>
+      <c r="U24" s="26"/>
+      <c r="Y24">
+        <v>1</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A25" s="24">
-        <v>16012001</v>
+        <v>16011001</v>
       </c>
       <c r="B25">
         <v>2</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E25" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="F25">
         <v>20</v>
       </c>
-      <c r="N25">
-        <v>1</v>
-      </c>
-      <c r="O25">
-        <v>1</v>
-      </c>
-      <c r="P25">
-        <v>1</v>
-      </c>
-      <c r="Q25">
-        <v>1</v>
-      </c>
-      <c r="Y25" t="s">
+      <c r="U25" s="26"/>
+      <c r="Y25">
+        <v>1</v>
+      </c>
+      <c r="Z25">
+        <v>1</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="A26" s="24">
+        <v>16011002</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>130</v>
+      </c>
+      <c r="E26" t="s">
+        <v>129</v>
+      </c>
+      <c r="F26">
+        <v>10</v>
+      </c>
+      <c r="G26" s="22"/>
+      <c r="U26" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="A27" s="24">
+        <v>16012001</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
         <v>108</v>
       </c>
+      <c r="E27" t="s">
+        <v>110</v>
+      </c>
+      <c r="F27">
+        <v>20</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+      <c r="U27" s="26"/>
+      <c r="AA27" t="s">
+        <v>106</v>
+      </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A26" s="25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="A28" s="25">
         <v>16020001</v>
       </c>
-      <c r="B26" s="22">
+      <c r="B28" s="22">
         <v>3</v>
       </c>
-      <c r="C26" s="22">
-        <v>1</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="C28" s="22">
+        <v>1</v>
+      </c>
+      <c r="D28" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="E28" t="s">
+        <v>120</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28" s="22"/>
+      <c r="H28">
+        <v>98</v>
+      </c>
+      <c r="U28" s="26"/>
+      <c r="AA28" s="22" t="s">
         <v>122</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26" s="22"/>
-      <c r="H26">
-        <v>98</v>
-      </c>
-      <c r="Y26" s="22" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B4:Y4 B16:E25 G16:Y25 B5:E14 G5:Y14 F5:F25">
-    <cfRule type="containsBlanks" dxfId="13" priority="4">
+  <conditionalFormatting sqref="B4:AA28">
+    <cfRule type="containsBlanks" dxfId="0" priority="6">
       <formula>LEN(TRIM(B4))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15:E15 G15:Y15">
-    <cfRule type="containsBlanks" dxfId="12" priority="3">
-      <formula>LEN(TRIM(B15))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B26:D26 F26:Y26">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(B26))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(E26))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add a trade based bless
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Bless.xlsx
+++ b/ConfigData/Xlsx/Bless.xlsx
@@ -15,11 +15,12 @@
     <sheet name="Bless" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="156">
   <si>
     <t>序列</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -561,6 +562,77 @@
   </si>
   <si>
     <t>rollfail3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>资源奖励系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardResMulti</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>矿工</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务获得资源（水晶、红宝石等）时可以获得额外一份</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>res1</t>
+  </si>
+  <si>
+    <t>交易时支付比例</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TradeNeedRate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>交易时得到比例</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TradeAddRate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>讨价还价</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>交易时可以少支持25%费用</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>-0.25</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>通胀</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>交易时需要多支持50%费用</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>double</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trade1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>traden1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -568,7 +640,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -755,8 +827,22 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="48">
+  <fills count="50">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1023,6 +1109,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1323,7 +1421,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1412,6 +1510,27 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="48" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="48" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="49" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1460,7 +1579,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill>
@@ -1469,7 +1588,18 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1497,6 +1627,9 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <font>
@@ -1804,22 +1937,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AA28" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9" headerRowCellStyle="百分比">
-  <autoFilter ref="A3:AA28"/>
-  <tableColumns count="27">
-    <tableColumn id="1" name="Id" dataDxfId="8"/>
-    <tableColumn id="14" name="Type" dataDxfId="7"/>
-    <tableColumn id="5" name="Level" dataDxfId="6"/>
-    <tableColumn id="2" name="Name" dataDxfId="5"/>
-    <tableColumn id="3" name="Descript" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AD31" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11" headerRowCellStyle="百分比">
+  <autoFilter ref="A3:AD31"/>
+  <tableColumns count="30">
+    <tableColumn id="1" name="Id" dataDxfId="10"/>
+    <tableColumn id="14" name="Type" dataDxfId="9"/>
+    <tableColumn id="5" name="Level" dataDxfId="8"/>
+    <tableColumn id="2" name="Name" dataDxfId="7"/>
+    <tableColumn id="3" name="Descript" dataDxfId="6"/>
     <tableColumn id="25" name="Round"/>
-    <tableColumn id="4" name="MoveFoodChange" dataDxfId="3"/>
+    <tableColumn id="4" name="MoveFoodChange" dataDxfId="5"/>
     <tableColumn id="20" name="MoveDistance"/>
     <tableColumn id="8" name="RewardGoldMulti"/>
     <tableColumn id="7" name="RewardFoodMulti"/>
     <tableColumn id="6" name="RewardHealthMulti"/>
     <tableColumn id="10" name="RewardMentalMulti"/>
     <tableColumn id="11" name="RewardExpMulti"/>
+    <tableColumn id="28" name="RewardResMulti"/>
     <tableColumn id="12" name="PunishGoldMulti"/>
     <tableColumn id="16" name="PunishFoodMulti"/>
     <tableColumn id="15" name="PunishHealthMulti"/>
@@ -1827,13 +1961,15 @@
     <tableColumn id="17" name="RollWinAddGold"/>
     <tableColumn id="18" name="RollFailSubHealth"/>
     <tableColumn id="27" name="RollAlwaysWinBig"/>
-    <tableColumn id="26" name="RollAlwaysFailBig" dataDxfId="1"/>
+    <tableColumn id="26" name="RollAlwaysFailBig" dataDxfId="4"/>
     <tableColumn id="19" name="FightLevelChange"/>
     <tableColumn id="21" name="FightWinAddHealth"/>
     <tableColumn id="24" name="FightWinAddExp"/>
     <tableColumn id="22" name="FightFailSubHealth"/>
     <tableColumn id="23" name="FightFailSubMental"/>
-    <tableColumn id="9" name="Icon" dataDxfId="2"/>
+    <tableColumn id="29" name="TradeNeedRate"/>
+    <tableColumn id="30" name="TradeAddRate"/>
+    <tableColumn id="9" name="Icon" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2160,10 +2296,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA28"/>
+  <dimension ref="A1:AD31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="AD14" sqref="AD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2173,13 +2309,13 @@
     <col min="5" max="5" width="34.375" customWidth="1"/>
     <col min="6" max="6" width="4.875" customWidth="1"/>
     <col min="7" max="8" width="4.5" customWidth="1"/>
-    <col min="9" max="19" width="3.875" customWidth="1"/>
-    <col min="20" max="21" width="4.5" customWidth="1"/>
-    <col min="22" max="26" width="3.875" customWidth="1"/>
-    <col min="30" max="30" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="20" width="3.875" customWidth="1"/>
+    <col min="21" max="22" width="4.5" customWidth="1"/>
+    <col min="23" max="29" width="3.875" customWidth="1"/>
+    <col min="33" max="33" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="66" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:30" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2219,50 +2355,59 @@
       <c r="M1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="O1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="P1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="27" t="s">
+      <c r="S1" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="S1" s="27" t="s">
+      <c r="T1" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="T1" s="27" t="s">
+      <c r="U1" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="U1" s="27" t="s">
+      <c r="V1" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="V1" s="14" t="s">
+      <c r="W1" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="W1" s="14" t="s">
+      <c r="X1" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="Y1" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="Y1" s="14" t="s">
+      <c r="Z1" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="AA1" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="AA1" s="10" t="s">
+      <c r="AB1" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="AC1" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="AD1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2302,8 +2447,8 @@
       <c r="M2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="17" t="s">
-        <v>29</v>
+      <c r="N2" s="16" t="s">
+        <v>139</v>
       </c>
       <c r="O2" s="17" t="s">
         <v>29</v>
@@ -2314,20 +2459,20 @@
       <c r="Q2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="R2" s="28" t="s">
+      <c r="R2" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="S2" s="28" t="s">
+      <c r="T2" s="28" t="s">
         <v>74</v>
-      </c>
-      <c r="T2" s="28" t="s">
-        <v>127</v>
       </c>
       <c r="U2" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="V2" s="18" t="s">
-        <v>83</v>
+      <c r="V2" s="28" t="s">
+        <v>127</v>
       </c>
       <c r="W2" s="18" t="s">
         <v>83</v>
@@ -2341,11 +2486,20 @@
       <c r="Z2" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AA2" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB2" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="AC2" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="AD2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -2385,50 +2539,59 @@
       <c r="M3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="O3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="P3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="Q3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="R3" s="29" t="s">
+      <c r="S3" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="S3" s="29" t="s">
+      <c r="T3" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="T3" s="29" t="s">
+      <c r="U3" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="U3" s="29" t="s">
+      <c r="V3" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="V3" s="7" t="s">
+      <c r="W3" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="W3" s="7" t="s">
+      <c r="X3" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="X3" s="7" t="s">
+      <c r="Y3" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="Y3" s="7" t="s">
+      <c r="Z3" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="Z3" s="7" t="s">
+      <c r="AA3" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="AA3" s="4" t="s">
+      <c r="AB3" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="AC3" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="AD3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A4" s="23">
         <v>16000001</v>
       </c>
@@ -2450,12 +2613,12 @@
       <c r="G4">
         <v>-1</v>
       </c>
-      <c r="U4" s="26"/>
-      <c r="AA4" t="s">
+      <c r="V4" s="26"/>
+      <c r="AD4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A5" s="23">
         <v>16000002</v>
       </c>
@@ -2477,12 +2640,12 @@
       <c r="I5">
         <v>1</v>
       </c>
-      <c r="U5" s="26"/>
-      <c r="AA5" t="s">
+      <c r="V5" s="26"/>
+      <c r="AD5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A6" s="23">
         <v>16000003</v>
       </c>
@@ -2504,12 +2667,12 @@
       <c r="J6">
         <v>1</v>
       </c>
-      <c r="U6" s="26"/>
-      <c r="AA6" t="s">
+      <c r="V6" s="26"/>
+      <c r="AD6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A7" s="23">
         <v>16000004</v>
       </c>
@@ -2531,12 +2694,12 @@
       <c r="K7">
         <v>1</v>
       </c>
-      <c r="U7" s="26"/>
-      <c r="AA7" t="s">
+      <c r="V7" s="26"/>
+      <c r="AD7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A8" s="23">
         <v>16000005</v>
       </c>
@@ -2558,12 +2721,12 @@
       <c r="L8">
         <v>1</v>
       </c>
-      <c r="U8" s="26"/>
-      <c r="AA8" t="s">
+      <c r="V8" s="26"/>
+      <c r="AD8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A9" s="23">
         <v>16000006</v>
       </c>
@@ -2585,12 +2748,12 @@
       <c r="M9">
         <v>1</v>
       </c>
-      <c r="U9" s="26"/>
-      <c r="AA9" t="s">
+      <c r="V9" s="26"/>
+      <c r="AD9" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A10" s="23">
         <v>16000007</v>
       </c>
@@ -2609,15 +2772,15 @@
       <c r="F10">
         <v>20</v>
       </c>
-      <c r="S10">
-        <v>1</v>
-      </c>
-      <c r="U10" s="26"/>
-      <c r="AA10" t="s">
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="V10" s="26"/>
+      <c r="AD10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A11" s="23">
         <v>16000008</v>
       </c>
@@ -2636,15 +2799,15 @@
       <c r="F11">
         <v>20</v>
       </c>
-      <c r="U11" s="26"/>
-      <c r="W11">
-        <v>1</v>
-      </c>
-      <c r="AA11" t="s">
+      <c r="V11" s="26"/>
+      <c r="X11">
+        <v>1</v>
+      </c>
+      <c r="AD11" s="35" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A12" s="23">
         <v>16000009</v>
       </c>
@@ -2666,44 +2829,42 @@
       <c r="H12">
         <v>1</v>
       </c>
-      <c r="U12" s="26"/>
-      <c r="AA12" s="22" t="s">
+      <c r="V12" s="26"/>
+      <c r="AD12" s="36" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A13" s="23">
-        <v>16001001</v>
+        <v>16000010</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>99</v>
-      </c>
-      <c r="E13" t="s">
-        <v>100</v>
+        <v>1</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>149</v>
       </c>
       <c r="F13">
         <v>20</v>
       </c>
-      <c r="U13" s="26"/>
-      <c r="W13">
-        <v>1</v>
-      </c>
-      <c r="X13">
-        <v>1</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>101</v>
+      <c r="G13" s="30"/>
+      <c r="V13" s="26"/>
+      <c r="AB13" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="AD13" s="36" t="s">
+        <v>154</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A14" s="23">
-        <v>16001002</v>
+        <v>16001001</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2712,143 +2873,148 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F14">
+        <v>20</v>
+      </c>
+      <c r="V14" s="26"/>
+      <c r="X14">
+        <v>1</v>
+      </c>
+      <c r="Y14">
+        <v>1</v>
+      </c>
+      <c r="AD14" s="35" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A15" s="23">
+        <v>16001002</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
         <v>134</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>135</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <v>10</v>
       </c>
-      <c r="T14" s="26" t="s">
+      <c r="U15" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="U14" s="26"/>
-      <c r="AA14" t="s">
+      <c r="V15" s="26"/>
+      <c r="AD15" s="35" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A15" s="23">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A16" s="23">
+        <v>16001003</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>141</v>
+      </c>
+      <c r="E16" t="s">
+        <v>142</v>
+      </c>
+      <c r="F16">
+        <v>20</v>
+      </c>
+      <c r="G16" s="30"/>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="U16" s="26"/>
+      <c r="V16" s="26"/>
+      <c r="AD16" s="36" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A17" s="23">
         <v>16002001</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
         <v>3</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D17" t="s">
         <v>107</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E17" t="s">
         <v>109</v>
-      </c>
-      <c r="F15">
-        <v>20</v>
-      </c>
-      <c r="G15" s="22"/>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <v>1</v>
-      </c>
-      <c r="U15" s="26"/>
-      <c r="AA15" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A16" s="23">
-        <v>16002002</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16" t="s">
-        <v>121</v>
-      </c>
-      <c r="E16" t="s">
-        <v>120</v>
-      </c>
-      <c r="F16">
-        <v>10</v>
-      </c>
-      <c r="H16">
-        <v>98</v>
-      </c>
-      <c r="U16" s="26"/>
-      <c r="AA16" s="22" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A17" s="24">
-        <v>16010001</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" t="s">
-        <v>18</v>
       </c>
       <c r="F17">
         <v>20</v>
       </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="U17" s="26"/>
-      <c r="AA17" t="s">
-        <v>19</v>
+      <c r="G17" s="22"/>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="V17" s="26"/>
+      <c r="AD17" s="35" t="s">
+        <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A18" s="24">
-        <v>16010002</v>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A18" s="23">
+        <v>16002002</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>121</v>
       </c>
       <c r="E18" t="s">
-        <v>47</v>
+        <v>120</v>
       </c>
       <c r="F18">
-        <v>20</v>
-      </c>
-      <c r="N18">
-        <v>1</v>
-      </c>
-      <c r="U18" s="26"/>
-      <c r="AA18" t="s">
-        <v>44</v>
+        <v>10</v>
+      </c>
+      <c r="H18">
+        <v>98</v>
+      </c>
+      <c r="V18" s="26"/>
+      <c r="AD18" s="36" t="s">
+        <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A19" s="24">
-        <v>16010003</v>
+        <v>16010001</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -2857,25 +3023,25 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="E19" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="F19">
         <v>20</v>
       </c>
-      <c r="O19">
-        <v>1</v>
-      </c>
-      <c r="U19" s="26"/>
-      <c r="AA19" t="s">
-        <v>49</v>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="V19" s="26"/>
+      <c r="AD19" s="35" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A20" s="24">
-        <v>16010004</v>
+        <v>16010002</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -2884,25 +3050,25 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F20">
         <v>20</v>
       </c>
-      <c r="P20">
-        <v>1</v>
-      </c>
-      <c r="U20" s="26"/>
-      <c r="AA20" t="s">
-        <v>58</v>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="V20" s="26"/>
+      <c r="AD20" s="35" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A21" s="24">
-        <v>16010005</v>
+        <v>16010003</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -2911,25 +3077,25 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="F21">
         <v>20</v>
       </c>
-      <c r="Q21">
-        <v>1</v>
-      </c>
-      <c r="U21" s="26"/>
-      <c r="AA21" t="s">
-        <v>62</v>
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="V21" s="26"/>
+      <c r="AD21" s="35" t="s">
+        <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A22" s="24">
-        <v>16010006</v>
+        <v>16010004</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -2938,25 +3104,25 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="E22" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="F22">
         <v>20</v>
       </c>
-      <c r="M22">
-        <v>-1</v>
-      </c>
-      <c r="U22" s="26"/>
-      <c r="AA22" t="s">
-        <v>67</v>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="V22" s="26"/>
+      <c r="AD22" s="35" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A23" s="24">
-        <v>16010007</v>
+        <v>16010005</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -2965,10 +3131,10 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="E23" t="s">
-        <v>124</v>
+        <v>65</v>
       </c>
       <c r="F23">
         <v>20</v>
@@ -2976,14 +3142,14 @@
       <c r="R23">
         <v>1</v>
       </c>
-      <c r="U23" s="26"/>
-      <c r="AA23" t="s">
-        <v>78</v>
+      <c r="V23" s="26"/>
+      <c r="AD23" s="35" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A24" s="24">
-        <v>16010008</v>
+        <v>16010006</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -2992,148 +3158,240 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="E24" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
       <c r="F24">
         <v>20</v>
       </c>
-      <c r="U24" s="26"/>
-      <c r="Y24">
-        <v>1</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>94</v>
+      <c r="M24">
+        <v>-1</v>
+      </c>
+      <c r="V24" s="26"/>
+      <c r="AD24" s="35" t="s">
+        <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A25" s="24">
-        <v>16011001</v>
+        <v>16010007</v>
       </c>
       <c r="B25">
         <v>2</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="E25" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="F25">
         <v>20</v>
       </c>
-      <c r="U25" s="26"/>
-      <c r="Y25">
-        <v>1</v>
-      </c>
-      <c r="Z25">
-        <v>1</v>
-      </c>
-      <c r="AA25" t="s">
-        <v>104</v>
+      <c r="S25">
+        <v>1</v>
+      </c>
+      <c r="V25" s="26"/>
+      <c r="AD25" s="35" t="s">
+        <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A26" s="24">
-        <v>16011002</v>
+        <v>16010008</v>
       </c>
       <c r="B26">
         <v>2</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>130</v>
+        <v>97</v>
       </c>
       <c r="E26" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="F26">
-        <v>10</v>
-      </c>
-      <c r="G26" s="22"/>
-      <c r="U26" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="AA26" t="s">
-        <v>137</v>
+        <v>20</v>
+      </c>
+      <c r="V26" s="26"/>
+      <c r="Z26">
+        <v>1</v>
+      </c>
+      <c r="AD26" s="35" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A27" s="24">
-        <v>16012001</v>
+        <v>16010009</v>
       </c>
       <c r="B27">
         <v>2</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>108</v>
-      </c>
-      <c r="E27" t="s">
-        <v>110</v>
+        <v>151</v>
+      </c>
+      <c r="E27" s="31" t="s">
+        <v>152</v>
       </c>
       <c r="F27">
         <v>20</v>
       </c>
-      <c r="N27">
-        <v>1</v>
-      </c>
-      <c r="O27">
-        <v>1</v>
-      </c>
-      <c r="P27">
-        <v>1</v>
-      </c>
-      <c r="Q27">
-        <v>1</v>
-      </c>
-      <c r="U27" s="26"/>
-      <c r="AA27" t="s">
+      <c r="G27" s="22"/>
+      <c r="V27" s="26"/>
+      <c r="AB27">
+        <v>0.5</v>
+      </c>
+      <c r="AD27" s="35" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A28" s="24">
+        <v>16011001</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>102</v>
+      </c>
+      <c r="E28" t="s">
+        <v>103</v>
+      </c>
+      <c r="F28">
+        <v>20</v>
+      </c>
+      <c r="V28" s="26"/>
+      <c r="Z28">
+        <v>1</v>
+      </c>
+      <c r="AA28">
+        <v>1</v>
+      </c>
+      <c r="AD28" s="35" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A29" s="24">
+        <v>16011002</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>130</v>
+      </c>
+      <c r="E29" t="s">
+        <v>129</v>
+      </c>
+      <c r="F29">
+        <v>10</v>
+      </c>
+      <c r="G29" s="22"/>
+      <c r="V29" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A30" s="24">
+        <v>16012001</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" t="s">
+        <v>110</v>
+      </c>
+      <c r="F30">
+        <v>20</v>
+      </c>
+      <c r="O30">
+        <v>1</v>
+      </c>
+      <c r="P30">
+        <v>1</v>
+      </c>
+      <c r="Q30">
+        <v>1</v>
+      </c>
+      <c r="R30">
+        <v>1</v>
+      </c>
+      <c r="V30" s="26"/>
+      <c r="AD30" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A28" s="25">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A31" s="25">
         <v>16020001</v>
       </c>
-      <c r="B28" s="22">
+      <c r="B31" s="22">
         <v>3</v>
       </c>
-      <c r="C28" s="22">
-        <v>1</v>
-      </c>
-      <c r="D28" s="22" t="s">
+      <c r="C31" s="22">
+        <v>1</v>
+      </c>
+      <c r="D31" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E31" t="s">
         <v>120</v>
       </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28" s="22"/>
-      <c r="H28">
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31" s="22"/>
+      <c r="H31">
         <v>98</v>
       </c>
-      <c r="U28" s="26"/>
-      <c r="AA28" s="22" t="s">
+      <c r="V31" s="26"/>
+      <c r="AD31" s="22" t="s">
         <v>122</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B4:AA28">
-    <cfRule type="containsBlanks" dxfId="0" priority="6">
+  <conditionalFormatting sqref="B4:AD26 B28:AD31 G27:AD27">
+    <cfRule type="containsBlanks" dxfId="2" priority="8">
       <formula>LEN(TRIM(B4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27:D27 F27">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(B27))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(E27))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finish some bless on test
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Bless.xlsx
+++ b/ConfigData/Xlsx/Bless.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="177">
   <si>
     <t>序列</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -204,10 +204,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>每次任务消耗金钱时需要支付额外一份</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>food1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -220,14 +216,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>每次任务获得食物时可以获得额外一份</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次任务消耗食物时需要支付额外一份</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>素食</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -236,14 +224,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>每次任务回复生命时可以获得额外一次回复</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次任务受到生命惩罚时会额外多触发一次</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>health1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -272,14 +252,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>每次任务回复精神时可以获得额外一次回复</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次任务受到精神惩罚时会额外多触发一次</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>发明</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -296,10 +268,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>每次任务获得经验时可以获得额外一次</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>无法通过任务获得经验</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -450,18 +418,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>每次任务成功会获得额外生命/精神/金钱/食物奖励</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次任务失败会获得受到生命/精神/金钱/食物惩罚</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次任务获得金钱时可以获得额外一份</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>MoveDistance</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -633,6 +589,134 @@
   </si>
   <si>
     <t>traden1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务奖励获得金钱时可以获得额外一份</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务奖励获得食物时可以获得额外一份</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务奖励回复生命时可以获得额外一次回复</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务奖励回复精神时可以获得额外一次回复</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务奖励获得经验时可以获得额外一次</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务惩罚金钱时需要支付额外一份</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务惩罚食物时需要支付额外一份</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务惩罚生命时会额外多触发一次</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务精神时会额外多触发一次</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务惩罚会获得受到额外的生命/精神/金钱/食物损失</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次任务奖励会获得额外生命/精神/金钱/食物加成</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>老手</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>能力考验时，所有的2分视为3分</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>能力考验2分调整</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestAdjustPointTwo</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>菜鸟</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>能力考验时，所有的2分视为1分</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>能力小球数量变化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestBallChange</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>能力小球同调</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestBallSynchonize</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>能力考验时，小球数量+1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>能力考验时，小球数量-1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>全能</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>苦手</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>能力考验时，所有小球初始速度和位置一致</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>偏激</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>test1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>test2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>testn1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>testn2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>testn3</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -842,7 +926,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="50">
+  <fills count="52">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1121,6 +1205,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1421,7 +1517,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1531,6 +1627,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="50" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="50" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="51" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1579,7 +1684,42 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="19">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1854,72 +1994,6 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
     <mruColors>
       <color rgb="FFB31D96"/>
       <color rgb="FFF577AD"/>
@@ -1937,16 +2011,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AD31" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11" headerRowCellStyle="百分比">
-  <autoFilter ref="A3:AD31"/>
-  <tableColumns count="30">
-    <tableColumn id="1" name="Id" dataDxfId="10"/>
-    <tableColumn id="14" name="Type" dataDxfId="9"/>
-    <tableColumn id="5" name="Level" dataDxfId="8"/>
-    <tableColumn id="2" name="Name" dataDxfId="7"/>
-    <tableColumn id="3" name="Descript" dataDxfId="6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AG36" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16" headerRowCellStyle="百分比">
+  <autoFilter ref="A3:AG36"/>
+  <tableColumns count="33">
+    <tableColumn id="1" name="Id" dataDxfId="15"/>
+    <tableColumn id="14" name="Type" dataDxfId="14"/>
+    <tableColumn id="5" name="Level" dataDxfId="13"/>
+    <tableColumn id="2" name="Name" dataDxfId="12"/>
+    <tableColumn id="3" name="Descript" dataDxfId="11"/>
     <tableColumn id="25" name="Round"/>
-    <tableColumn id="4" name="MoveFoodChange" dataDxfId="5"/>
+    <tableColumn id="4" name="MoveFoodChange" dataDxfId="10"/>
     <tableColumn id="20" name="MoveDistance"/>
     <tableColumn id="8" name="RewardGoldMulti"/>
     <tableColumn id="7" name="RewardFoodMulti"/>
@@ -1961,7 +2035,7 @@
     <tableColumn id="17" name="RollWinAddGold"/>
     <tableColumn id="18" name="RollFailSubHealth"/>
     <tableColumn id="27" name="RollAlwaysWinBig"/>
-    <tableColumn id="26" name="RollAlwaysFailBig" dataDxfId="4"/>
+    <tableColumn id="26" name="RollAlwaysFailBig" dataDxfId="9"/>
     <tableColumn id="19" name="FightLevelChange"/>
     <tableColumn id="21" name="FightWinAddHealth"/>
     <tableColumn id="24" name="FightWinAddExp"/>
@@ -1969,7 +2043,10 @@
     <tableColumn id="23" name="FightFailSubMental"/>
     <tableColumn id="29" name="TradeNeedRate"/>
     <tableColumn id="30" name="TradeAddRate"/>
-    <tableColumn id="9" name="Icon" dataDxfId="3"/>
+    <tableColumn id="31" name="TestAdjustPointTwo"/>
+    <tableColumn id="32" name="TestBallChange"/>
+    <tableColumn id="33" name="TestBallSynchonize"/>
+    <tableColumn id="9" name="Icon" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1983,7 +2060,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2296,10 +2373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD31"/>
+  <dimension ref="A1:AG36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD14" sqref="AD14"/>
+    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="AG34" sqref="AG34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2311,11 +2388,12 @@
     <col min="7" max="8" width="4.5" customWidth="1"/>
     <col min="9" max="20" width="3.875" customWidth="1"/>
     <col min="21" max="22" width="4.5" customWidth="1"/>
-    <col min="23" max="29" width="3.875" customWidth="1"/>
-    <col min="33" max="33" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="31" width="3.875" customWidth="1"/>
+    <col min="32" max="32" width="4.625" customWidth="1"/>
+    <col min="36" max="36" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="66" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:33" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2332,13 +2410,13 @@
         <v>2</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="G1" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>24</v>
@@ -2356,7 +2434,7 @@
         <v>28</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="O1" s="13" t="s">
         <v>30</v>
@@ -2371,43 +2449,52 @@
         <v>33</v>
       </c>
       <c r="S1" s="27" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="T1" s="27" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="U1" s="27" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="V1" s="27" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="W1" s="14" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="X1" s="14" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="Y1" s="14" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="Z1" s="14" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="AA1" s="14" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="AB1" s="32" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="AC1" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="AD1" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="AD1" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE1" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="AF1" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="AG1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2448,7 +2535,7 @@
         <v>29</v>
       </c>
       <c r="N2" s="16" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="O2" s="17" t="s">
         <v>29</v>
@@ -2463,43 +2550,52 @@
         <v>29</v>
       </c>
       <c r="S2" s="28" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="T2" s="28" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="U2" s="28" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="V2" s="28" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="W2" s="18" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="X2" s="18" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="Y2" s="18" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="Z2" s="18" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="AA2" s="18" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="AB2" s="33" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="AC2" s="33" t="s">
-        <v>153</v>
-      </c>
-      <c r="AD2" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD2" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE2" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF2" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -2516,13 +2612,13 @@
         <v>9</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>42</v>
@@ -2540,7 +2636,7 @@
         <v>37</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>38</v>
@@ -2555,43 +2651,52 @@
         <v>41</v>
       </c>
       <c r="S3" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="T3" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="U3" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="V3" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="W3" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="T3" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="U3" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="V3" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="W3" s="7" t="s">
+      <c r="X3" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y3" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="X3" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y3" s="7" t="s">
-        <v>92</v>
-      </c>
       <c r="Z3" s="7" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="AA3" s="7" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="AB3" s="34" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="AC3" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="AD3" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="AD3" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="AE3" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="AF3" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="AG3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A4" s="23">
         <v>16000001</v>
       </c>
@@ -2614,11 +2719,11 @@
         <v>-1</v>
       </c>
       <c r="V4" s="26"/>
-      <c r="AD4" t="s">
+      <c r="AG4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A5" s="23">
         <v>16000002</v>
       </c>
@@ -2632,7 +2737,7 @@
         <v>45</v>
       </c>
       <c r="E5" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="F5">
         <v>20</v>
@@ -2641,11 +2746,11 @@
         <v>1</v>
       </c>
       <c r="V5" s="26"/>
-      <c r="AD5" t="s">
+      <c r="AG5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A6" s="23">
         <v>16000003</v>
       </c>
@@ -2656,10 +2761,10 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>146</v>
       </c>
       <c r="F6">
         <v>20</v>
@@ -2668,11 +2773,11 @@
         <v>1</v>
       </c>
       <c r="V6" s="26"/>
-      <c r="AD6" t="s">
-        <v>48</v>
+      <c r="AG6" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A7" s="23">
         <v>16000004</v>
       </c>
@@ -2683,10 +2788,10 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>147</v>
       </c>
       <c r="F7">
         <v>20</v>
@@ -2695,11 +2800,11 @@
         <v>1</v>
       </c>
       <c r="V7" s="26"/>
-      <c r="AD7" t="s">
-        <v>57</v>
+      <c r="AG7" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A8" s="23">
         <v>16000005</v>
       </c>
@@ -2710,10 +2815,10 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>148</v>
       </c>
       <c r="F8">
         <v>20</v>
@@ -2722,11 +2827,11 @@
         <v>1</v>
       </c>
       <c r="V8" s="26"/>
-      <c r="AD8" t="s">
-        <v>61</v>
+      <c r="AG8" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A9" s="23">
         <v>16000006</v>
       </c>
@@ -2737,10 +2842,10 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>149</v>
       </c>
       <c r="F9">
         <v>20</v>
@@ -2749,11 +2854,11 @@
         <v>1</v>
       </c>
       <c r="V9" s="26"/>
-      <c r="AD9" t="s">
-        <v>68</v>
+      <c r="AG9" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A10" s="23">
         <v>16000007</v>
       </c>
@@ -2764,10 +2869,10 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E10" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="F10">
         <v>20</v>
@@ -2776,11 +2881,11 @@
         <v>1</v>
       </c>
       <c r="V10" s="26"/>
-      <c r="AD10" t="s">
-        <v>79</v>
+      <c r="AG10" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A11" s="23">
         <v>16000008</v>
       </c>
@@ -2791,10 +2896,10 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E11" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F11">
         <v>20</v>
@@ -2803,11 +2908,11 @@
       <c r="X11">
         <v>1</v>
       </c>
-      <c r="AD11" s="35" t="s">
-        <v>93</v>
+      <c r="AG11" s="35" t="s">
+        <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A12" s="23">
         <v>16000009</v>
       </c>
@@ -2818,10 +2923,10 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="E12" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="F12">
         <v>10</v>
@@ -2830,11 +2935,11 @@
         <v>1</v>
       </c>
       <c r="V12" s="26"/>
-      <c r="AD12" s="36" t="s">
-        <v>116</v>
+      <c r="AG12" s="36" t="s">
+        <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A13" s="23">
         <v>16000010</v>
       </c>
@@ -2845,10 +2950,10 @@
         <v>1</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="F13">
         <v>20</v>
@@ -2856,45 +2961,44 @@
       <c r="G13" s="30"/>
       <c r="V13" s="26"/>
       <c r="AB13" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="AD13" s="36" t="s">
-        <v>154</v>
+        <v>139</v>
+      </c>
+      <c r="AG13" s="36" t="s">
+        <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A14" s="23">
-        <v>16001001</v>
+        <v>16000011</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14" t="s">
-        <v>99</v>
-      </c>
-      <c r="E14" t="s">
-        <v>100</v>
+        <v>1</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>157</v>
       </c>
       <c r="F14">
         <v>20</v>
       </c>
+      <c r="G14" s="22"/>
       <c r="V14" s="26"/>
-      <c r="X14">
-        <v>1</v>
-      </c>
-      <c r="Y14">
-        <v>1</v>
-      </c>
-      <c r="AD14" s="35" t="s">
-        <v>101</v>
+      <c r="AB14" s="26"/>
+      <c r="AD14">
+        <v>1</v>
+      </c>
+      <c r="AG14" s="22" t="s">
+        <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A15" s="23">
-        <v>16001002</v>
+        <v>16001001</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2903,25 +3007,28 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>134</v>
+        <v>91</v>
       </c>
       <c r="E15" t="s">
-        <v>135</v>
+        <v>92</v>
       </c>
       <c r="F15">
-        <v>10</v>
-      </c>
-      <c r="U15" s="26" t="s">
-        <v>131</v>
+        <v>20</v>
       </c>
       <c r="V15" s="26"/>
-      <c r="AD15" s="35" t="s">
-        <v>136</v>
+      <c r="X15">
+        <v>1</v>
+      </c>
+      <c r="Y15">
+        <v>1</v>
+      </c>
+      <c r="AG15" s="35" t="s">
+        <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A16" s="23">
-        <v>16001003</v>
+        <v>16001002</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2930,145 +3037,147 @@
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="E16" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="F16">
-        <v>20</v>
-      </c>
-      <c r="G16" s="30"/>
-      <c r="N16">
-        <v>1</v>
-      </c>
-      <c r="U16" s="26"/>
+        <v>10</v>
+      </c>
+      <c r="U16" s="26" t="s">
+        <v>120</v>
+      </c>
       <c r="V16" s="26"/>
-      <c r="AD16" s="36" t="s">
-        <v>143</v>
+      <c r="AG16" s="35" t="s">
+        <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A17" s="23">
-        <v>16002001</v>
+        <v>16001003</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
       <c r="E17" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="F17">
         <v>20</v>
       </c>
-      <c r="G17" s="22"/>
-      <c r="I17">
-        <v>1</v>
-      </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-      <c r="L17">
-        <v>1</v>
-      </c>
+      <c r="G17" s="30"/>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="U17" s="26"/>
       <c r="V17" s="26"/>
-      <c r="AD17" s="35" t="s">
-        <v>105</v>
+      <c r="AG17" s="36" t="s">
+        <v>132</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A18" s="23">
-        <v>16002002</v>
+        <v>16001004</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>168</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="F18">
+        <v>20</v>
+      </c>
+      <c r="G18" s="22"/>
+      <c r="U18" s="26"/>
+      <c r="V18" s="26"/>
+      <c r="AE18">
+        <v>1</v>
+      </c>
+      <c r="AG18" s="22" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A19" s="23">
+        <v>16002001</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
         <v>3</v>
       </c>
-      <c r="D18" t="s">
-        <v>121</v>
-      </c>
-      <c r="E18" t="s">
-        <v>120</v>
-      </c>
-      <c r="F18">
-        <v>10</v>
-      </c>
-      <c r="H18">
-        <v>98</v>
-      </c>
-      <c r="V18" s="26"/>
-      <c r="AD18" s="36" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="A19" s="24">
-        <v>16010001</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="E19" t="s">
-        <v>18</v>
+        <v>155</v>
       </c>
       <c r="F19">
         <v>20</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="22"/>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
         <v>1</v>
       </c>
       <c r="V19" s="26"/>
-      <c r="AD19" s="35" t="s">
-        <v>19</v>
+      <c r="AG19" s="35" t="s">
+        <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="A20" s="24">
-        <v>16010002</v>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A20" s="23">
+        <v>16002002</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>110</v>
       </c>
       <c r="E20" t="s">
-        <v>47</v>
+        <v>109</v>
       </c>
       <c r="F20">
-        <v>20</v>
-      </c>
-      <c r="O20">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="H20">
+        <v>98</v>
       </c>
       <c r="V20" s="26"/>
-      <c r="AD20" s="35" t="s">
-        <v>44</v>
+      <c r="AG20" s="36" t="s">
+        <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A21" s="24">
-        <v>16010003</v>
+        <v>16010001</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -3077,25 +3186,25 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="F21">
         <v>20</v>
       </c>
-      <c r="P21">
+      <c r="G21">
         <v>1</v>
       </c>
       <c r="V21" s="26"/>
-      <c r="AD21" s="35" t="s">
-        <v>49</v>
+      <c r="AG21" s="35" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A22" s="24">
-        <v>16010004</v>
+        <v>16010002</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -3104,25 +3213,25 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
+        <v>150</v>
       </c>
       <c r="F22">
         <v>20</v>
       </c>
-      <c r="Q22">
+      <c r="O22">
         <v>1</v>
       </c>
       <c r="V22" s="26"/>
-      <c r="AD22" s="35" t="s">
-        <v>58</v>
+      <c r="AG22" s="35" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A23" s="24">
-        <v>16010005</v>
+        <v>16010003</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -3131,25 +3240,25 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="E23" t="s">
-        <v>65</v>
+        <v>151</v>
       </c>
       <c r="F23">
         <v>20</v>
       </c>
-      <c r="R23">
+      <c r="P23">
         <v>1</v>
       </c>
       <c r="V23" s="26"/>
-      <c r="AD23" s="35" t="s">
-        <v>62</v>
+      <c r="AG23" s="35" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A24" s="24">
-        <v>16010006</v>
+        <v>16010004</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -3158,25 +3267,25 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="E24" t="s">
-        <v>71</v>
+        <v>152</v>
       </c>
       <c r="F24">
         <v>20</v>
       </c>
-      <c r="M24">
-        <v>-1</v>
+      <c r="Q24">
+        <v>1</v>
       </c>
       <c r="V24" s="26"/>
-      <c r="AD24" s="35" t="s">
-        <v>67</v>
+      <c r="AG24" s="35" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A25" s="24">
-        <v>16010007</v>
+        <v>16010005</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -3185,25 +3294,25 @@
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="E25" t="s">
-        <v>124</v>
+        <v>153</v>
       </c>
       <c r="F25">
         <v>20</v>
       </c>
-      <c r="S25">
+      <c r="R25">
         <v>1</v>
       </c>
       <c r="V25" s="26"/>
-      <c r="AD25" s="35" t="s">
-        <v>78</v>
+      <c r="AG25" s="35" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A26" s="24">
-        <v>16010008</v>
+        <v>16010006</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -3212,25 +3321,25 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="E26" t="s">
-        <v>98</v>
+        <v>63</v>
       </c>
       <c r="F26">
         <v>20</v>
       </c>
+      <c r="M26">
+        <v>-1</v>
+      </c>
       <c r="V26" s="26"/>
-      <c r="Z26">
-        <v>1</v>
-      </c>
-      <c r="AD26" s="35" t="s">
-        <v>94</v>
+      <c r="AG26" s="35" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A27" s="24">
-        <v>16010009</v>
+        <v>16010007</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -3239,38 +3348,37 @@
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>151</v>
-      </c>
-      <c r="E27" s="31" t="s">
-        <v>152</v>
+        <v>73</v>
+      </c>
+      <c r="E27" t="s">
+        <v>113</v>
       </c>
       <c r="F27">
         <v>20</v>
       </c>
-      <c r="G27" s="22"/>
+      <c r="S27">
+        <v>1</v>
+      </c>
       <c r="V27" s="26"/>
-      <c r="AB27">
-        <v>0.5</v>
-      </c>
-      <c r="AD27" s="35" t="s">
-        <v>155</v>
+      <c r="AG27" s="35" t="s">
+        <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A28" s="24">
-        <v>16011001</v>
+        <v>16010008</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="E28" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="F28">
         <v>20</v>
@@ -3279,119 +3387,283 @@
       <c r="Z28">
         <v>1</v>
       </c>
-      <c r="AA28">
-        <v>1</v>
-      </c>
-      <c r="AD28" s="35" t="s">
-        <v>104</v>
+      <c r="AG28" s="35" t="s">
+        <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A29" s="24">
-        <v>16011002</v>
+        <v>16010009</v>
       </c>
       <c r="B29">
         <v>2</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>130</v>
-      </c>
-      <c r="E29" t="s">
-        <v>129</v>
+        <v>140</v>
+      </c>
+      <c r="E29" s="31" t="s">
+        <v>141</v>
       </c>
       <c r="F29">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G29" s="22"/>
-      <c r="V29" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="AD29" t="s">
-        <v>137</v>
+      <c r="V29" s="26"/>
+      <c r="AB29">
+        <v>0.5</v>
+      </c>
+      <c r="AG29" s="35" t="s">
+        <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A30" s="24">
-        <v>16012001</v>
+        <v>16010010</v>
       </c>
       <c r="B30">
         <v>2</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>108</v>
-      </c>
-      <c r="E30" t="s">
-        <v>110</v>
+        <v>160</v>
+      </c>
+      <c r="E30" s="31" t="s">
+        <v>161</v>
       </c>
       <c r="F30">
         <v>20</v>
       </c>
-      <c r="O30">
-        <v>1</v>
-      </c>
-      <c r="P30">
-        <v>1</v>
-      </c>
-      <c r="Q30">
-        <v>1</v>
-      </c>
-      <c r="R30">
-        <v>1</v>
-      </c>
+      <c r="G30" s="22"/>
       <c r="V30" s="26"/>
-      <c r="AD30" t="s">
-        <v>106</v>
+      <c r="AD30">
+        <v>-1</v>
+      </c>
+      <c r="AG30" s="22" t="s">
+        <v>174</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="A31" s="25">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A31" s="24">
+        <v>16010011</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>171</v>
+      </c>
+      <c r="E31" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="F31">
+        <v>20</v>
+      </c>
+      <c r="G31" s="22"/>
+      <c r="V31" s="26"/>
+      <c r="AF31" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG31" s="22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A32" s="24">
+        <v>16011001</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>94</v>
+      </c>
+      <c r="E32" t="s">
+        <v>95</v>
+      </c>
+      <c r="F32">
+        <v>20</v>
+      </c>
+      <c r="V32" s="26"/>
+      <c r="Z32">
+        <v>1</v>
+      </c>
+      <c r="AA32">
+        <v>1</v>
+      </c>
+      <c r="AG32" s="35" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A33" s="24">
+        <v>16011002</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>119</v>
+      </c>
+      <c r="E33" t="s">
+        <v>118</v>
+      </c>
+      <c r="F33">
+        <v>10</v>
+      </c>
+      <c r="G33" s="22"/>
+      <c r="V33" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A34" s="24">
+        <v>16011003</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>169</v>
+      </c>
+      <c r="E34" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="F34">
+        <v>20</v>
+      </c>
+      <c r="G34" s="22"/>
+      <c r="V34" s="26"/>
+      <c r="AE34">
+        <v>-1</v>
+      </c>
+      <c r="AG34" s="22" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A35" s="24">
+        <v>16012001</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35" t="s">
+        <v>100</v>
+      </c>
+      <c r="E35" t="s">
+        <v>154</v>
+      </c>
+      <c r="F35">
+        <v>20</v>
+      </c>
+      <c r="O35">
+        <v>1</v>
+      </c>
+      <c r="P35">
+        <v>1</v>
+      </c>
+      <c r="Q35">
+        <v>1</v>
+      </c>
+      <c r="R35">
+        <v>1</v>
+      </c>
+      <c r="V35" s="26"/>
+      <c r="AG35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A36" s="25">
         <v>16020001</v>
       </c>
-      <c r="B31" s="22">
+      <c r="B36" s="22">
         <v>3</v>
       </c>
-      <c r="C31" s="22">
-        <v>1</v>
-      </c>
-      <c r="D31" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="E31" t="s">
-        <v>120</v>
-      </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-      <c r="G31" s="22"/>
-      <c r="H31">
+      <c r="C36" s="22">
+        <v>1</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="E36" t="s">
+        <v>109</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36" s="22"/>
+      <c r="H36">
         <v>98</v>
       </c>
-      <c r="V31" s="26"/>
-      <c r="AD31" s="22" t="s">
-        <v>122</v>
+      <c r="V36" s="26"/>
+      <c r="AG36" s="22" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B4:AD26 B28:AD31 G27:AD27">
-    <cfRule type="containsBlanks" dxfId="2" priority="8">
+  <conditionalFormatting sqref="B30:F30 B4:AG17 B19:AG28 G18:AG18 B35:AG36 G34:AG34 B32:AG33 G29:AG31">
+    <cfRule type="containsBlanks" dxfId="7" priority="13">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B27:D27 F27">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(B27))=0</formula>
+  <conditionalFormatting sqref="B29:D29 F29">
+    <cfRule type="containsBlanks" dxfId="6" priority="7">
+      <formula>LEN(TRIM(B29))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E27">
+  <conditionalFormatting sqref="E29">
+    <cfRule type="containsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(E29))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:D18 F18">
+    <cfRule type="containsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(B18))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(E18))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34:D34 F34">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(B34))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(E34))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B31:F31">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(E27))=0</formula>
+      <formula>LEN(TRIM(B31))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
support a new type bless
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Bless.xlsx
+++ b/ConfigData/Xlsx/Bless.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="182">
   <si>
     <t>序列</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -717,6 +717,26 @@
   </si>
   <si>
     <t>testn3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>移动消耗等同食物的生命</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MoveCostHp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>重伤</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次移动会受到等同食物消耗的生命损失</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>moven1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -915,6 +935,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -2011,9 +2032,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AG36" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16" headerRowCellStyle="百分比">
-  <autoFilter ref="A3:AG36"/>
-  <tableColumns count="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AH37" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16" headerRowCellStyle="百分比">
+  <autoFilter ref="A3:AH37"/>
+  <tableColumns count="34">
     <tableColumn id="1" name="Id" dataDxfId="15"/>
     <tableColumn id="14" name="Type" dataDxfId="14"/>
     <tableColumn id="5" name="Level" dataDxfId="13"/>
@@ -2022,6 +2043,7 @@
     <tableColumn id="25" name="Round"/>
     <tableColumn id="4" name="MoveFoodChange" dataDxfId="10"/>
     <tableColumn id="20" name="MoveDistance"/>
+    <tableColumn id="34" name="MoveCostHp"/>
     <tableColumn id="8" name="RewardGoldMulti"/>
     <tableColumn id="7" name="RewardFoodMulti"/>
     <tableColumn id="6" name="RewardHealthMulti"/>
@@ -2373,10 +2395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG36"/>
+  <dimension ref="A1:AH37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="AG34" sqref="AG34"/>
+    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
+      <selection activeCell="AH36" sqref="AH36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2385,15 +2407,15 @@
     <col min="2" max="3" width="5.125" customWidth="1"/>
     <col min="5" max="5" width="34.375" customWidth="1"/>
     <col min="6" max="6" width="4.875" customWidth="1"/>
-    <col min="7" max="8" width="4.5" customWidth="1"/>
-    <col min="9" max="20" width="3.875" customWidth="1"/>
-    <col min="21" max="22" width="4.5" customWidth="1"/>
-    <col min="23" max="31" width="3.875" customWidth="1"/>
-    <col min="32" max="32" width="4.625" customWidth="1"/>
-    <col min="36" max="36" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="4.5" customWidth="1"/>
+    <col min="10" max="21" width="3.875" customWidth="1"/>
+    <col min="22" max="23" width="4.5" customWidth="1"/>
+    <col min="24" max="32" width="3.875" customWidth="1"/>
+    <col min="33" max="33" width="4.625" customWidth="1"/>
+    <col min="37" max="37" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="66" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:34" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2418,83 +2440,86 @@
       <c r="H1" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="P1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="27" t="s">
+      <c r="T1" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="T1" s="27" t="s">
+      <c r="U1" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="U1" s="27" t="s">
+      <c r="V1" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="W1" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="W1" s="14" t="s">
+      <c r="X1" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="Y1" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="Y1" s="14" t="s">
+      <c r="Z1" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="AA1" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="AA1" s="14" t="s">
+      <c r="AB1" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="AB1" s="32" t="s">
+      <c r="AC1" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="AC1" s="32" t="s">
+      <c r="AD1" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="AD1" s="37" t="s">
+      <c r="AE1" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="AE1" s="37" t="s">
+      <c r="AF1" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="AF1" s="37" t="s">
+      <c r="AG1" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="AG1" s="10" t="s">
+      <c r="AH1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2519,8 +2544,8 @@
       <c r="H2" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="16" t="s">
-        <v>29</v>
+      <c r="I2" s="15" t="s">
+        <v>116</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>29</v>
@@ -2535,10 +2560,10 @@
         <v>29</v>
       </c>
       <c r="N2" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="16" t="s">
         <v>128</v>
-      </c>
-      <c r="O2" s="17" t="s">
-        <v>29</v>
       </c>
       <c r="P2" s="17" t="s">
         <v>29</v>
@@ -2549,20 +2574,20 @@
       <c r="R2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="S2" s="28" t="s">
+      <c r="S2" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="T2" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="T2" s="28" t="s">
+      <c r="U2" s="28" t="s">
         <v>66</v>
-      </c>
-      <c r="U2" s="28" t="s">
-        <v>116</v>
       </c>
       <c r="V2" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="W2" s="18" t="s">
-        <v>75</v>
+      <c r="W2" s="28" t="s">
+        <v>116</v>
       </c>
       <c r="X2" s="18" t="s">
         <v>75</v>
@@ -2576,26 +2601,29 @@
       <c r="AA2" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="AB2" s="33" t="s">
-        <v>142</v>
+      <c r="AB2" s="18" t="s">
+        <v>75</v>
       </c>
       <c r="AC2" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="AD2" s="38" t="s">
-        <v>5</v>
+      <c r="AD2" s="33" t="s">
+        <v>142</v>
       </c>
       <c r="AE2" s="38" t="s">
         <v>5</v>
       </c>
       <c r="AF2" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG2" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AH2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -2620,83 +2648,86 @@
       <c r="H3" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="P3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="Q3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="S3" s="29" t="s">
+      <c r="T3" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="T3" s="29" t="s">
+      <c r="U3" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="U3" s="29" t="s">
+      <c r="V3" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="V3" s="29" t="s">
+      <c r="W3" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="W3" s="7" t="s">
+      <c r="X3" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="X3" s="7" t="s">
+      <c r="Y3" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="Y3" s="7" t="s">
+      <c r="Z3" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="Z3" s="7" t="s">
+      <c r="AA3" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="AA3" s="7" t="s">
+      <c r="AB3" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="AB3" s="34" t="s">
+      <c r="AC3" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="AC3" s="34" t="s">
+      <c r="AD3" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="AD3" s="39" t="s">
+      <c r="AE3" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="AE3" s="39" t="s">
+      <c r="AF3" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="AF3" s="39" t="s">
+      <c r="AG3" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="AG3" s="4" t="s">
+      <c r="AH3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A4" s="23">
         <v>16000001</v>
       </c>
@@ -2718,12 +2749,12 @@
       <c r="G4">
         <v>-1</v>
       </c>
-      <c r="V4" s="26"/>
-      <c r="AG4" t="s">
+      <c r="W4" s="26"/>
+      <c r="AH4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A5" s="23">
         <v>16000002</v>
       </c>
@@ -2742,15 +2773,15 @@
       <c r="F5">
         <v>20</v>
       </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="V5" s="26"/>
-      <c r="AG5" t="s">
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="W5" s="26"/>
+      <c r="AH5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A6" s="23">
         <v>16000003</v>
       </c>
@@ -2769,15 +2800,15 @@
       <c r="F6">
         <v>20</v>
       </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="V6" s="26"/>
-      <c r="AG6" t="s">
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="W6" s="26"/>
+      <c r="AH6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A7" s="23">
         <v>16000004</v>
       </c>
@@ -2796,15 +2827,15 @@
       <c r="F7">
         <v>20</v>
       </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="V7" s="26"/>
-      <c r="AG7" t="s">
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="W7" s="26"/>
+      <c r="AH7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A8" s="23">
         <v>16000005</v>
       </c>
@@ -2823,15 +2854,15 @@
       <c r="F8">
         <v>20</v>
       </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
-      <c r="V8" s="26"/>
-      <c r="AG8" t="s">
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="W8" s="26"/>
+      <c r="AH8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A9" s="23">
         <v>16000006</v>
       </c>
@@ -2850,15 +2881,15 @@
       <c r="F9">
         <v>20</v>
       </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
-      <c r="V9" s="26"/>
-      <c r="AG9" t="s">
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="W9" s="26"/>
+      <c r="AH9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A10" s="23">
         <v>16000007</v>
       </c>
@@ -2877,15 +2908,15 @@
       <c r="F10">
         <v>20</v>
       </c>
-      <c r="T10">
-        <v>1</v>
-      </c>
-      <c r="V10" s="26"/>
-      <c r="AG10" t="s">
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="W10" s="26"/>
+      <c r="AH10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A11" s="23">
         <v>16000008</v>
       </c>
@@ -2904,15 +2935,15 @@
       <c r="F11">
         <v>20</v>
       </c>
-      <c r="V11" s="26"/>
-      <c r="X11">
-        <v>1</v>
-      </c>
-      <c r="AG11" s="35" t="s">
+      <c r="W11" s="26"/>
+      <c r="Y11">
+        <v>1</v>
+      </c>
+      <c r="AH11" s="35" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A12" s="23">
         <v>16000009</v>
       </c>
@@ -2934,12 +2965,12 @@
       <c r="H12">
         <v>1</v>
       </c>
-      <c r="V12" s="26"/>
-      <c r="AG12" s="36" t="s">
+      <c r="W12" s="26"/>
+      <c r="AH12" s="36" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A13" s="23">
         <v>16000010</v>
       </c>
@@ -2959,15 +2990,15 @@
         <v>20</v>
       </c>
       <c r="G13" s="30"/>
-      <c r="V13" s="26"/>
-      <c r="AB13" s="26" t="s">
+      <c r="W13" s="26"/>
+      <c r="AC13" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="AG13" s="36" t="s">
+      <c r="AH13" s="36" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A14" s="23">
         <v>16000011</v>
       </c>
@@ -2987,16 +3018,16 @@
         <v>20</v>
       </c>
       <c r="G14" s="22"/>
-      <c r="V14" s="26"/>
-      <c r="AB14" s="26"/>
-      <c r="AD14">
-        <v>1</v>
-      </c>
-      <c r="AG14" s="22" t="s">
+      <c r="W14" s="26"/>
+      <c r="AC14" s="26"/>
+      <c r="AE14">
+        <v>1</v>
+      </c>
+      <c r="AH14" s="22" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A15" s="23">
         <v>16001001</v>
       </c>
@@ -3015,18 +3046,18 @@
       <c r="F15">
         <v>20</v>
       </c>
-      <c r="V15" s="26"/>
-      <c r="X15">
-        <v>1</v>
-      </c>
+      <c r="W15" s="26"/>
       <c r="Y15">
         <v>1</v>
       </c>
-      <c r="AG15" s="35" t="s">
+      <c r="Z15">
+        <v>1</v>
+      </c>
+      <c r="AH15" s="35" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A16" s="23">
         <v>16001002</v>
       </c>
@@ -3045,15 +3076,15 @@
       <c r="F16">
         <v>10</v>
       </c>
-      <c r="U16" s="26" t="s">
+      <c r="V16" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="V16" s="26"/>
-      <c r="AG16" s="35" t="s">
+      <c r="W16" s="26"/>
+      <c r="AH16" s="35" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A17" s="23">
         <v>16001003</v>
       </c>
@@ -3073,16 +3104,16 @@
         <v>20</v>
       </c>
       <c r="G17" s="30"/>
-      <c r="N17">
-        <v>1</v>
-      </c>
-      <c r="U17" s="26"/>
+      <c r="O17">
+        <v>1</v>
+      </c>
       <c r="V17" s="26"/>
-      <c r="AG17" s="36" t="s">
+      <c r="W17" s="26"/>
+      <c r="AH17" s="36" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A18" s="23">
         <v>16001004</v>
       </c>
@@ -3102,16 +3133,16 @@
         <v>20</v>
       </c>
       <c r="G18" s="22"/>
-      <c r="U18" s="26"/>
       <c r="V18" s="26"/>
-      <c r="AE18">
-        <v>1</v>
-      </c>
-      <c r="AG18" s="22" t="s">
+      <c r="W18" s="26"/>
+      <c r="AF18">
+        <v>1</v>
+      </c>
+      <c r="AH18" s="22" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A19" s="23">
         <v>16002001</v>
       </c>
@@ -3131,9 +3162,6 @@
         <v>20</v>
       </c>
       <c r="G19" s="22"/>
-      <c r="I19">
-        <v>1</v>
-      </c>
       <c r="J19">
         <v>1</v>
       </c>
@@ -3143,12 +3171,15 @@
       <c r="L19">
         <v>1</v>
       </c>
-      <c r="V19" s="26"/>
-      <c r="AG19" s="35" t="s">
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="W19" s="26"/>
+      <c r="AH19" s="35" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A20" s="23">
         <v>16002002</v>
       </c>
@@ -3170,12 +3201,12 @@
       <c r="H20">
         <v>98</v>
       </c>
-      <c r="V20" s="26"/>
-      <c r="AG20" s="36" t="s">
+      <c r="W20" s="26"/>
+      <c r="AH20" s="36" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A21" s="24">
         <v>16010001</v>
       </c>
@@ -3197,12 +3228,12 @@
       <c r="G21">
         <v>1</v>
       </c>
-      <c r="V21" s="26"/>
-      <c r="AG21" s="35" t="s">
+      <c r="W21" s="26"/>
+      <c r="AH21" s="35" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A22" s="24">
         <v>16010002</v>
       </c>
@@ -3221,15 +3252,15 @@
       <c r="F22">
         <v>20</v>
       </c>
-      <c r="O22">
-        <v>1</v>
-      </c>
-      <c r="V22" s="26"/>
-      <c r="AG22" s="35" t="s">
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="W22" s="26"/>
+      <c r="AH22" s="35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A23" s="24">
         <v>16010003</v>
       </c>
@@ -3248,15 +3279,15 @@
       <c r="F23">
         <v>20</v>
       </c>
-      <c r="P23">
-        <v>1</v>
-      </c>
-      <c r="V23" s="26"/>
-      <c r="AG23" s="35" t="s">
+      <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="W23" s="26"/>
+      <c r="AH23" s="35" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A24" s="24">
         <v>16010004</v>
       </c>
@@ -3275,15 +3306,15 @@
       <c r="F24">
         <v>20</v>
       </c>
-      <c r="Q24">
-        <v>1</v>
-      </c>
-      <c r="V24" s="26"/>
-      <c r="AG24" s="35" t="s">
+      <c r="R24">
+        <v>1</v>
+      </c>
+      <c r="W24" s="26"/>
+      <c r="AH24" s="35" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A25" s="24">
         <v>16010005</v>
       </c>
@@ -3302,15 +3333,15 @@
       <c r="F25">
         <v>20</v>
       </c>
-      <c r="R25">
-        <v>1</v>
-      </c>
-      <c r="V25" s="26"/>
-      <c r="AG25" s="35" t="s">
+      <c r="S25">
+        <v>1</v>
+      </c>
+      <c r="W25" s="26"/>
+      <c r="AH25" s="35" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A26" s="24">
         <v>16010006</v>
       </c>
@@ -3329,15 +3360,15 @@
       <c r="F26">
         <v>20</v>
       </c>
-      <c r="M26">
+      <c r="N26">
         <v>-1</v>
       </c>
-      <c r="V26" s="26"/>
-      <c r="AG26" s="35" t="s">
+      <c r="W26" s="26"/>
+      <c r="AH26" s="35" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A27" s="24">
         <v>16010007</v>
       </c>
@@ -3356,15 +3387,15 @@
       <c r="F27">
         <v>20</v>
       </c>
-      <c r="S27">
-        <v>1</v>
-      </c>
-      <c r="V27" s="26"/>
-      <c r="AG27" s="35" t="s">
+      <c r="T27">
+        <v>1</v>
+      </c>
+      <c r="W27" s="26"/>
+      <c r="AH27" s="35" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A28" s="24">
         <v>16010008</v>
       </c>
@@ -3383,15 +3414,15 @@
       <c r="F28">
         <v>20</v>
       </c>
-      <c r="V28" s="26"/>
-      <c r="Z28">
-        <v>1</v>
-      </c>
-      <c r="AG28" s="35" t="s">
+      <c r="W28" s="26"/>
+      <c r="AA28">
+        <v>1</v>
+      </c>
+      <c r="AH28" s="35" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A29" s="24">
         <v>16010009</v>
       </c>
@@ -3411,15 +3442,15 @@
         <v>20</v>
       </c>
       <c r="G29" s="22"/>
-      <c r="V29" s="26"/>
-      <c r="AB29">
+      <c r="W29" s="26"/>
+      <c r="AC29">
         <v>0.5</v>
       </c>
-      <c r="AG29" s="35" t="s">
+      <c r="AH29" s="35" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A30" s="24">
         <v>16010010</v>
       </c>
@@ -3439,15 +3470,15 @@
         <v>20</v>
       </c>
       <c r="G30" s="22"/>
-      <c r="V30" s="26"/>
-      <c r="AD30">
+      <c r="W30" s="26"/>
+      <c r="AE30">
         <v>-1</v>
       </c>
-      <c r="AG30" s="22" t="s">
+      <c r="AH30" s="22" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A31" s="24">
         <v>16010011</v>
       </c>
@@ -3467,15 +3498,15 @@
         <v>20</v>
       </c>
       <c r="G31" s="22"/>
-      <c r="V31" s="26"/>
-      <c r="AF31" s="26" t="s">
+      <c r="W31" s="26"/>
+      <c r="AG31" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="AG31" s="22" t="s">
+      <c r="AH31" s="22" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A32" s="24">
         <v>16011001</v>
       </c>
@@ -3494,18 +3525,18 @@
       <c r="F32">
         <v>20</v>
       </c>
-      <c r="V32" s="26"/>
-      <c r="Z32">
-        <v>1</v>
-      </c>
+      <c r="W32" s="26"/>
       <c r="AA32">
         <v>1</v>
       </c>
-      <c r="AG32" s="35" t="s">
+      <c r="AB32">
+        <v>1</v>
+      </c>
+      <c r="AH32" s="35" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A33" s="24">
         <v>16011002</v>
       </c>
@@ -3525,14 +3556,14 @@
         <v>10</v>
       </c>
       <c r="G33" s="22"/>
-      <c r="V33" s="26" t="s">
+      <c r="W33" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="AG33" t="s">
+      <c r="AH33" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A34" s="24">
         <v>16011003</v>
       </c>
@@ -3552,15 +3583,15 @@
         <v>20</v>
       </c>
       <c r="G34" s="22"/>
-      <c r="V34" s="26"/>
-      <c r="AE34">
+      <c r="W34" s="26"/>
+      <c r="AF34">
         <v>-1</v>
       </c>
-      <c r="AG34" s="22" t="s">
+      <c r="AH34" s="22" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A35" s="24">
         <v>16012001</v>
       </c>
@@ -3579,9 +3610,6 @@
       <c r="F35">
         <v>20</v>
       </c>
-      <c r="O35">
-        <v>1</v>
-      </c>
       <c r="P35">
         <v>1</v>
       </c>
@@ -3591,42 +3619,73 @@
       <c r="R35">
         <v>1</v>
       </c>
-      <c r="V35" s="26"/>
-      <c r="AG35" t="s">
+      <c r="S35">
+        <v>1</v>
+      </c>
+      <c r="W35" s="26"/>
+      <c r="AH35" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.15">
-      <c r="A36" s="25">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.15">
+      <c r="A36" s="24">
+        <v>16012002</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="F36">
+        <v>20</v>
+      </c>
+      <c r="G36" s="22"/>
+      <c r="I36" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="W36" s="26"/>
+      <c r="AH36" s="22" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="37" spans="1:34" x14ac:dyDescent="0.15">
+      <c r="A37" s="25">
         <v>16020001</v>
       </c>
-      <c r="B36" s="22">
+      <c r="B37" s="22">
         <v>3</v>
       </c>
-      <c r="C36" s="22">
-        <v>1</v>
-      </c>
-      <c r="D36" s="22" t="s">
+      <c r="C37" s="22">
+        <v>1</v>
+      </c>
+      <c r="D37" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E37" t="s">
         <v>109</v>
       </c>
-      <c r="F36">
-        <v>1</v>
-      </c>
-      <c r="G36" s="22"/>
-      <c r="H36">
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37" s="22"/>
+      <c r="H37">
         <v>98</v>
       </c>
-      <c r="V36" s="26"/>
-      <c r="AG36" s="22" t="s">
+      <c r="W37" s="26"/>
+      <c r="AH37" s="22" t="s">
         <v>111</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B30:F30 B4:AG17 B19:AG28 G18:AG18 B35:AG36 G34:AG34 B32:AG33 G29:AG31">
+  <conditionalFormatting sqref="B30:F30 B4:AH17 B19:AH28 G18:AH18 G34:AH34 B32:AH33 G29:AH31 B35:AH37">
     <cfRule type="containsBlanks" dxfId="7" priority="13">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
use bless name not id by scene quest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Bless.xlsx
+++ b/ConfigData/Xlsx/Bless.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="185">
   <si>
     <t>序列</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -737,6 +737,18 @@
   </si>
   <si>
     <t>moven1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>英文名</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ename</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1705,7 +1717,43 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2032,16 +2080,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AH37" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16" headerRowCellStyle="百分比">
-  <autoFilter ref="A3:AH37"/>
-  <tableColumns count="34">
-    <tableColumn id="1" name="Id" dataDxfId="15"/>
-    <tableColumn id="14" name="Type" dataDxfId="14"/>
-    <tableColumn id="5" name="Level" dataDxfId="13"/>
-    <tableColumn id="2" name="Name" dataDxfId="12"/>
-    <tableColumn id="3" name="Descript" dataDxfId="11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AI37" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18" headerRowCellStyle="百分比">
+  <autoFilter ref="A3:AI37"/>
+  <tableColumns count="35">
+    <tableColumn id="1" name="Id" dataDxfId="17"/>
+    <tableColumn id="14" name="Type" dataDxfId="16"/>
+    <tableColumn id="5" name="Level" dataDxfId="15"/>
+    <tableColumn id="2" name="Name" dataDxfId="14"/>
+    <tableColumn id="35" name="Ename" dataDxfId="0"/>
+    <tableColumn id="3" name="Descript" dataDxfId="13"/>
     <tableColumn id="25" name="Round"/>
-    <tableColumn id="4" name="MoveFoodChange" dataDxfId="10"/>
+    <tableColumn id="4" name="MoveFoodChange" dataDxfId="12"/>
     <tableColumn id="20" name="MoveDistance"/>
     <tableColumn id="34" name="MoveCostHp"/>
     <tableColumn id="8" name="RewardGoldMulti"/>
@@ -2057,7 +2106,7 @@
     <tableColumn id="17" name="RollWinAddGold"/>
     <tableColumn id="18" name="RollFailSubHealth"/>
     <tableColumn id="27" name="RollAlwaysWinBig"/>
-    <tableColumn id="26" name="RollAlwaysFailBig" dataDxfId="9"/>
+    <tableColumn id="26" name="RollAlwaysFailBig" dataDxfId="11"/>
     <tableColumn id="19" name="FightLevelChange"/>
     <tableColumn id="21" name="FightWinAddHealth"/>
     <tableColumn id="24" name="FightWinAddExp"/>
@@ -2068,7 +2117,7 @@
     <tableColumn id="31" name="TestAdjustPointTwo"/>
     <tableColumn id="32" name="TestBallChange"/>
     <tableColumn id="33" name="TestBallSynchonize"/>
-    <tableColumn id="9" name="Icon" dataDxfId="8"/>
+    <tableColumn id="9" name="Icon" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2395,27 +2444,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH37"/>
+  <dimension ref="A1:AI37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
-      <selection activeCell="AH36" sqref="AH36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="5.125" customWidth="1"/>
-    <col min="5" max="5" width="34.375" customWidth="1"/>
-    <col min="6" max="6" width="4.875" customWidth="1"/>
-    <col min="7" max="9" width="4.5" customWidth="1"/>
-    <col min="10" max="21" width="3.875" customWidth="1"/>
-    <col min="22" max="23" width="4.5" customWidth="1"/>
-    <col min="24" max="32" width="3.875" customWidth="1"/>
-    <col min="33" max="33" width="4.625" customWidth="1"/>
-    <col min="37" max="37" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.375" customWidth="1"/>
+    <col min="6" max="6" width="34.375" customWidth="1"/>
+    <col min="7" max="7" width="4.875" customWidth="1"/>
+    <col min="8" max="10" width="4.5" customWidth="1"/>
+    <col min="11" max="22" width="3.875" customWidth="1"/>
+    <col min="23" max="24" width="4.5" customWidth="1"/>
+    <col min="25" max="33" width="3.875" customWidth="1"/>
+    <col min="34" max="34" width="4.625" customWidth="1"/>
+    <col min="38" max="38" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="66" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:35" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2429,97 +2479,100 @@
         <v>1</v>
       </c>
       <c r="E1" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="27" t="s">
+      <c r="U1" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="U1" s="27" t="s">
+      <c r="V1" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="W1" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="W1" s="27" t="s">
+      <c r="X1" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="Y1" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="Y1" s="14" t="s">
+      <c r="Z1" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="AA1" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="AA1" s="14" t="s">
+      <c r="AB1" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="AB1" s="14" t="s">
+      <c r="AC1" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="AC1" s="32" t="s">
+      <c r="AD1" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="AD1" s="32" t="s">
+      <c r="AE1" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="AE1" s="37" t="s">
+      <c r="AF1" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="AF1" s="37" t="s">
+      <c r="AG1" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="AG1" s="37" t="s">
+      <c r="AH1" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="AH1" s="10" t="s">
+      <c r="AI1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2533,22 +2586,22 @@
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="G2" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="I2" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="J2" s="15" t="s">
         <v>116</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>29</v>
       </c>
       <c r="K2" s="16" t="s">
         <v>29</v>
@@ -2563,10 +2616,10 @@
         <v>29</v>
       </c>
       <c r="O2" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="16" t="s">
         <v>128</v>
-      </c>
-      <c r="P2" s="17" t="s">
-        <v>29</v>
       </c>
       <c r="Q2" s="17" t="s">
         <v>29</v>
@@ -2577,20 +2630,20 @@
       <c r="S2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="T2" s="28" t="s">
+      <c r="T2" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="U2" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="U2" s="28" t="s">
+      <c r="V2" s="28" t="s">
         <v>66</v>
-      </c>
-      <c r="V2" s="28" t="s">
-        <v>116</v>
       </c>
       <c r="W2" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="X2" s="18" t="s">
-        <v>75</v>
+      <c r="X2" s="28" t="s">
+        <v>116</v>
       </c>
       <c r="Y2" s="18" t="s">
         <v>75</v>
@@ -2604,26 +2657,29 @@
       <c r="AB2" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="AC2" s="33" t="s">
-        <v>142</v>
+      <c r="AC2" s="18" t="s">
+        <v>75</v>
       </c>
       <c r="AD2" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="AE2" s="38" t="s">
-        <v>5</v>
+      <c r="AE2" s="33" t="s">
+        <v>142</v>
       </c>
       <c r="AF2" s="38" t="s">
         <v>5</v>
       </c>
       <c r="AG2" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH2" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AI2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -2637,97 +2693,100 @@
         <v>8</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="G3" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="Q3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="T3" s="29" t="s">
+      <c r="U3" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="U3" s="29" t="s">
+      <c r="V3" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="V3" s="29" t="s">
+      <c r="W3" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="W3" s="29" t="s">
+      <c r="X3" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="X3" s="7" t="s">
+      <c r="Y3" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="Y3" s="7" t="s">
+      <c r="Z3" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="Z3" s="7" t="s">
+      <c r="AA3" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="AA3" s="7" t="s">
+      <c r="AB3" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="AB3" s="7" t="s">
+      <c r="AC3" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="AC3" s="34" t="s">
+      <c r="AD3" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="AD3" s="34" t="s">
+      <c r="AE3" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="AE3" s="39" t="s">
+      <c r="AF3" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="AF3" s="39" t="s">
+      <c r="AG3" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="AG3" s="39" t="s">
+      <c r="AH3" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="AH3" s="4" t="s">
+      <c r="AI3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A4" s="23">
         <v>16000001</v>
       </c>
@@ -2741,20 +2800,23 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>20</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>-1</v>
       </c>
-      <c r="W4" s="26"/>
-      <c r="AH4" t="s">
+      <c r="X4" s="26"/>
+      <c r="AI4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A5" s="23">
         <v>16000002</v>
       </c>
@@ -2768,20 +2830,23 @@
         <v>45</v>
       </c>
       <c r="E5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
         <v>145</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>20</v>
       </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="W5" s="26"/>
-      <c r="AH5" t="s">
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="X5" s="26"/>
+      <c r="AI5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A6" s="23">
         <v>16000003</v>
       </c>
@@ -2795,20 +2860,23 @@
         <v>50</v>
       </c>
       <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
         <v>146</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>20</v>
       </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="W6" s="26"/>
-      <c r="AH6" t="s">
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="X6" s="26"/>
+      <c r="AI6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A7" s="23">
         <v>16000004</v>
       </c>
@@ -2822,20 +2890,23 @@
         <v>51</v>
       </c>
       <c r="E7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" t="s">
         <v>147</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>20</v>
       </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="W7" s="26"/>
-      <c r="AH7" t="s">
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="X7" s="26"/>
+      <c r="AI7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A8" s="23">
         <v>16000005</v>
       </c>
@@ -2849,20 +2920,23 @@
         <v>55</v>
       </c>
       <c r="E8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" t="s">
         <v>148</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>20</v>
       </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="W8" s="26"/>
-      <c r="AH8" t="s">
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="X8" s="26"/>
+      <c r="AI8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A9" s="23">
         <v>16000006</v>
       </c>
@@ -2876,20 +2950,23 @@
         <v>59</v>
       </c>
       <c r="E9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" t="s">
         <v>149</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>20</v>
       </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-      <c r="W9" s="26"/>
-      <c r="AH9" t="s">
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="X9" s="26"/>
+      <c r="AI9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A10" s="23">
         <v>16000007</v>
       </c>
@@ -2903,20 +2980,23 @@
         <v>72</v>
       </c>
       <c r="E10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" t="s">
         <v>114</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>20</v>
       </c>
-      <c r="U10">
-        <v>1</v>
-      </c>
-      <c r="W10" s="26"/>
-      <c r="AH10" t="s">
+      <c r="V10">
+        <v>1</v>
+      </c>
+      <c r="X10" s="26"/>
+      <c r="AI10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A11" s="23">
         <v>16000008</v>
       </c>
@@ -2929,21 +3009,24 @@
       <c r="D11" t="s">
         <v>87</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" t="s">
         <v>88</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>20</v>
       </c>
-      <c r="W11" s="26"/>
-      <c r="Y11">
-        <v>1</v>
-      </c>
-      <c r="AH11" s="35" t="s">
+      <c r="X11" s="26"/>
+      <c r="Z11">
+        <v>1</v>
+      </c>
+      <c r="AI11" s="35" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A12" s="23">
         <v>16000009</v>
       </c>
@@ -2956,21 +3039,24 @@
       <c r="D12" t="s">
         <v>106</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="F12" t="s">
         <v>107</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>10</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="W12" s="26"/>
-      <c r="AH12" s="36" t="s">
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="X12" s="26"/>
+      <c r="AI12" s="36" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A13" s="23">
         <v>16000010</v>
       </c>
@@ -2983,22 +3069,25 @@
       <c r="D13" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="F13" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>20</v>
       </c>
-      <c r="G13" s="30"/>
-      <c r="W13" s="26"/>
-      <c r="AC13" s="26" t="s">
+      <c r="H13" s="30"/>
+      <c r="X13" s="26"/>
+      <c r="AD13" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="AH13" s="36" t="s">
+      <c r="AI13" s="36" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A14" s="23">
         <v>16000011</v>
       </c>
@@ -3011,23 +3100,26 @@
       <c r="D14" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="F14" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>20</v>
       </c>
-      <c r="G14" s="22"/>
-      <c r="W14" s="26"/>
-      <c r="AC14" s="26"/>
-      <c r="AE14">
-        <v>1</v>
-      </c>
-      <c r="AH14" s="22" t="s">
+      <c r="H14" s="22"/>
+      <c r="X14" s="26"/>
+      <c r="AD14" s="26"/>
+      <c r="AF14">
+        <v>1</v>
+      </c>
+      <c r="AI14" s="22" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A15" s="23">
         <v>16001001</v>
       </c>
@@ -3040,24 +3132,27 @@
       <c r="D15" t="s">
         <v>91</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" t="s">
         <v>92</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>20</v>
       </c>
-      <c r="W15" s="26"/>
-      <c r="Y15">
-        <v>1</v>
-      </c>
+      <c r="X15" s="26"/>
       <c r="Z15">
         <v>1</v>
       </c>
-      <c r="AH15" s="35" t="s">
+      <c r="AA15">
+        <v>1</v>
+      </c>
+      <c r="AI15" s="35" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A16" s="23">
         <v>16001002</v>
       </c>
@@ -3070,21 +3165,24 @@
       <c r="D16" t="s">
         <v>123</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="F16" t="s">
         <v>124</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>10</v>
       </c>
-      <c r="V16" s="26" t="s">
+      <c r="W16" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="W16" s="26"/>
-      <c r="AH16" s="35" t="s">
+      <c r="X16" s="26"/>
+      <c r="AI16" s="35" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A17" s="23">
         <v>16001003</v>
       </c>
@@ -3097,23 +3195,26 @@
       <c r="D17" t="s">
         <v>130</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="F17" t="s">
         <v>131</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>20</v>
       </c>
-      <c r="G17" s="30"/>
-      <c r="O17">
-        <v>1</v>
-      </c>
-      <c r="V17" s="26"/>
+      <c r="H17" s="30"/>
+      <c r="P17">
+        <v>1</v>
+      </c>
       <c r="W17" s="26"/>
-      <c r="AH17" s="36" t="s">
+      <c r="X17" s="26"/>
+      <c r="AI17" s="36" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A18" s="23">
         <v>16001004</v>
       </c>
@@ -3126,23 +3227,26 @@
       <c r="D18" t="s">
         <v>168</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="F18" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>20</v>
       </c>
-      <c r="G18" s="22"/>
-      <c r="V18" s="26"/>
+      <c r="H18" s="22"/>
       <c r="W18" s="26"/>
-      <c r="AF18">
-        <v>1</v>
-      </c>
-      <c r="AH18" s="22" t="s">
+      <c r="X18" s="26"/>
+      <c r="AG18">
+        <v>1</v>
+      </c>
+      <c r="AI18" s="22" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A19" s="23">
         <v>16002001</v>
       </c>
@@ -3155,16 +3259,16 @@
       <c r="D19" t="s">
         <v>99</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="F19" t="s">
         <v>155</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>20</v>
       </c>
-      <c r="G19" s="22"/>
-      <c r="J19">
-        <v>1</v>
-      </c>
+      <c r="H19" s="22"/>
       <c r="K19">
         <v>1</v>
       </c>
@@ -3174,12 +3278,15 @@
       <c r="M19">
         <v>1</v>
       </c>
-      <c r="W19" s="26"/>
-      <c r="AH19" s="35" t="s">
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="X19" s="26"/>
+      <c r="AI19" s="35" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A20" s="23">
         <v>16002002</v>
       </c>
@@ -3192,21 +3299,24 @@
       <c r="D20" t="s">
         <v>110</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="F20" t="s">
         <v>109</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>10</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>98</v>
       </c>
-      <c r="W20" s="26"/>
-      <c r="AH20" s="36" t="s">
+      <c r="X20" s="26"/>
+      <c r="AI20" s="36" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A21" s="24">
         <v>16010001</v>
       </c>
@@ -3219,21 +3329,24 @@
       <c r="D21" t="s">
         <v>16</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" t="s">
         <v>18</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>20</v>
       </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="W21" s="26"/>
-      <c r="AH21" s="35" t="s">
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="X21" s="26"/>
+      <c r="AI21" s="35" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A22" s="24">
         <v>16010002</v>
       </c>
@@ -3246,21 +3359,24 @@
       <c r="D22" t="s">
         <v>46</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" t="s">
         <v>150</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>20</v>
       </c>
-      <c r="P22">
-        <v>1</v>
-      </c>
-      <c r="W22" s="26"/>
-      <c r="AH22" s="35" t="s">
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="X22" s="26"/>
+      <c r="AI22" s="35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A23" s="24">
         <v>16010003</v>
       </c>
@@ -3273,21 +3389,24 @@
       <c r="D23" t="s">
         <v>49</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" t="s">
         <v>151</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>20</v>
       </c>
-      <c r="Q23">
-        <v>1</v>
-      </c>
-      <c r="W23" s="26"/>
-      <c r="AH23" s="35" t="s">
+      <c r="R23">
+        <v>1</v>
+      </c>
+      <c r="X23" s="26"/>
+      <c r="AI23" s="35" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A24" s="24">
         <v>16010004</v>
       </c>
@@ -3300,21 +3419,24 @@
       <c r="D24" t="s">
         <v>54</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" t="s">
         <v>152</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>20</v>
       </c>
-      <c r="R24">
-        <v>1</v>
-      </c>
-      <c r="W24" s="26"/>
-      <c r="AH24" s="35" t="s">
+      <c r="S24">
+        <v>1</v>
+      </c>
+      <c r="X24" s="26"/>
+      <c r="AI24" s="35" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A25" s="24">
         <v>16010005</v>
       </c>
@@ -3327,21 +3449,24 @@
       <c r="D25" t="s">
         <v>58</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" t="s">
         <v>153</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>20</v>
       </c>
-      <c r="S25">
-        <v>1</v>
-      </c>
-      <c r="W25" s="26"/>
-      <c r="AH25" s="35" t="s">
+      <c r="T25">
+        <v>1</v>
+      </c>
+      <c r="X25" s="26"/>
+      <c r="AI25" s="35" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A26" s="24">
         <v>16010006</v>
       </c>
@@ -3354,21 +3479,24 @@
       <c r="D26" t="s">
         <v>62</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" t="s">
         <v>63</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>20</v>
       </c>
-      <c r="N26">
+      <c r="O26">
         <v>-1</v>
       </c>
-      <c r="W26" s="26"/>
-      <c r="AH26" s="35" t="s">
+      <c r="X26" s="26"/>
+      <c r="AI26" s="35" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A27" s="24">
         <v>16010007</v>
       </c>
@@ -3381,21 +3509,24 @@
       <c r="D27" t="s">
         <v>73</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" t="s">
         <v>113</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>20</v>
       </c>
-      <c r="T27">
-        <v>1</v>
-      </c>
-      <c r="W27" s="26"/>
-      <c r="AH27" s="35" t="s">
+      <c r="U27">
+        <v>1</v>
+      </c>
+      <c r="X27" s="26"/>
+      <c r="AI27" s="35" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A28" s="24">
         <v>16010008</v>
       </c>
@@ -3408,21 +3539,24 @@
       <c r="D28" t="s">
         <v>89</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="F28" t="s">
         <v>90</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>20</v>
       </c>
-      <c r="W28" s="26"/>
-      <c r="AA28">
-        <v>1</v>
-      </c>
-      <c r="AH28" s="35" t="s">
+      <c r="X28" s="26"/>
+      <c r="AB28">
+        <v>1</v>
+      </c>
+      <c r="AI28" s="35" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A29" s="24">
         <v>16010009</v>
       </c>
@@ -3435,22 +3569,25 @@
       <c r="D29" t="s">
         <v>140</v>
       </c>
-      <c r="E29" s="31" t="s">
+      <c r="E29" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="F29" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>20</v>
       </c>
-      <c r="G29" s="22"/>
-      <c r="W29" s="26"/>
-      <c r="AC29">
+      <c r="H29" s="22"/>
+      <c r="X29" s="26"/>
+      <c r="AD29">
         <v>0.5</v>
       </c>
-      <c r="AH29" s="35" t="s">
+      <c r="AI29" s="35" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A30" s="24">
         <v>16010010</v>
       </c>
@@ -3463,22 +3600,25 @@
       <c r="D30" t="s">
         <v>160</v>
       </c>
-      <c r="E30" s="31" t="s">
+      <c r="E30" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="F30" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>20</v>
       </c>
-      <c r="G30" s="22"/>
-      <c r="W30" s="26"/>
-      <c r="AE30">
+      <c r="H30" s="22"/>
+      <c r="X30" s="26"/>
+      <c r="AF30">
         <v>-1</v>
       </c>
-      <c r="AH30" s="22" t="s">
+      <c r="AI30" s="22" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A31" s="24">
         <v>16010011</v>
       </c>
@@ -3491,22 +3631,25 @@
       <c r="D31" t="s">
         <v>171</v>
       </c>
-      <c r="E31" s="31" t="s">
+      <c r="E31" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="F31" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>20</v>
       </c>
-      <c r="G31" s="22"/>
-      <c r="W31" s="26"/>
-      <c r="AG31" s="26" t="s">
+      <c r="H31" s="22"/>
+      <c r="X31" s="26"/>
+      <c r="AH31" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="AH31" s="22" t="s">
+      <c r="AI31" s="22" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A32" s="24">
         <v>16011001</v>
       </c>
@@ -3519,24 +3662,27 @@
       <c r="D32" t="s">
         <v>94</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="F32" t="s">
         <v>95</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>20</v>
       </c>
-      <c r="W32" s="26"/>
-      <c r="AA32">
-        <v>1</v>
-      </c>
+      <c r="X32" s="26"/>
       <c r="AB32">
         <v>1</v>
       </c>
-      <c r="AH32" s="35" t="s">
+      <c r="AC32">
+        <v>1</v>
+      </c>
+      <c r="AI32" s="35" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A33" s="24">
         <v>16011002</v>
       </c>
@@ -3550,20 +3696,23 @@
         <v>119</v>
       </c>
       <c r="E33" t="s">
+        <v>126</v>
+      </c>
+      <c r="F33" t="s">
         <v>118</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>10</v>
       </c>
-      <c r="G33" s="22"/>
-      <c r="W33" s="26" t="s">
+      <c r="H33" s="22"/>
+      <c r="X33" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="AH33" t="s">
+      <c r="AI33" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A34" s="24">
         <v>16011003</v>
       </c>
@@ -3576,22 +3725,25 @@
       <c r="D34" t="s">
         <v>169</v>
       </c>
-      <c r="E34" s="31" t="s">
+      <c r="E34" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="F34" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>20</v>
       </c>
-      <c r="G34" s="22"/>
-      <c r="W34" s="26"/>
-      <c r="AF34">
+      <c r="H34" s="22"/>
+      <c r="X34" s="26"/>
+      <c r="AG34">
         <v>-1</v>
       </c>
-      <c r="AH34" s="22" t="s">
+      <c r="AI34" s="22" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A35" s="24">
         <v>16012001</v>
       </c>
@@ -3605,14 +3757,14 @@
         <v>100</v>
       </c>
       <c r="E35" t="s">
+        <v>98</v>
+      </c>
+      <c r="F35" t="s">
         <v>154</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>20</v>
       </c>
-      <c r="P35">
-        <v>1</v>
-      </c>
       <c r="Q35">
         <v>1</v>
       </c>
@@ -3622,12 +3774,15 @@
       <c r="S35">
         <v>1</v>
       </c>
-      <c r="W35" s="26"/>
-      <c r="AH35" t="s">
+      <c r="T35">
+        <v>1</v>
+      </c>
+      <c r="X35" s="26"/>
+      <c r="AI35" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A36" s="24">
         <v>16012002</v>
       </c>
@@ -3641,21 +3796,24 @@
         <v>179</v>
       </c>
       <c r="E36" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="F36" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>20</v>
       </c>
-      <c r="G36" s="22"/>
-      <c r="I36" s="26" t="s">
+      <c r="H36" s="22"/>
+      <c r="J36" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="W36" s="26"/>
-      <c r="AH36" s="22" t="s">
+      <c r="X36" s="26"/>
+      <c r="AI36" s="22" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A37" s="25">
         <v>16020001</v>
       </c>
@@ -3668,61 +3826,69 @@
       <c r="D37" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F37" t="s">
         <v>109</v>
       </c>
-      <c r="F37">
-        <v>1</v>
-      </c>
-      <c r="G37" s="22"/>
-      <c r="H37">
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37" s="22"/>
+      <c r="I37">
         <v>98</v>
       </c>
-      <c r="W37" s="26"/>
-      <c r="AH37" s="22" t="s">
+      <c r="X37" s="26"/>
+      <c r="AI37" s="22" t="s">
         <v>111</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B30:F30 B4:AH17 B19:AH28 G18:AH18 G34:AH34 B32:AH33 G29:AH31 B35:AH37">
-    <cfRule type="containsBlanks" dxfId="7" priority="13">
+  <conditionalFormatting sqref="B30:D30 B4:D17 B19:D28 H18:AI18 H34:AI34 B32:D33 H29:AI31 B35:D37 F35:AI37 F32:AI33 F19:AI28 F4:AI17 F30:G30">
+    <cfRule type="containsBlanks" dxfId="9" priority="14">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29:D29 F29">
-    <cfRule type="containsBlanks" dxfId="6" priority="7">
+  <conditionalFormatting sqref="B29:D29 G29">
+    <cfRule type="containsBlanks" dxfId="8" priority="8">
       <formula>LEN(TRIM(B29))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="containsBlanks" dxfId="5" priority="6">
-      <formula>LEN(TRIM(E29))=0</formula>
+  <conditionalFormatting sqref="F29">
+    <cfRule type="containsBlanks" dxfId="7" priority="7">
+      <formula>LEN(TRIM(F29))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B18:D18 F18">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
+  <conditionalFormatting sqref="B18:D18 G18">
+    <cfRule type="containsBlanks" dxfId="6" priority="6">
       <formula>LEN(TRIM(B18))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E18">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
-      <formula>LEN(TRIM(E18))=0</formula>
+  <conditionalFormatting sqref="F18">
+    <cfRule type="containsBlanks" dxfId="5" priority="5">
+      <formula>LEN(TRIM(F18))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B34:D34 F34">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
+  <conditionalFormatting sqref="B34:D34 G34">
+    <cfRule type="containsBlanks" dxfId="4" priority="4">
       <formula>LEN(TRIM(B34))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E34">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(E34))=0</formula>
+  <conditionalFormatting sqref="F34">
+    <cfRule type="containsBlanks" dxfId="3" priority="3">
+      <formula>LEN(TRIM(F34))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B31:F31">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+  <conditionalFormatting sqref="B31:D31 F31:G31">
+    <cfRule type="containsBlanks" dxfId="2" priority="2">
       <formula>LEN(TRIM(B31))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E37">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(E4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
a new curse type
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Bless.xlsx
+++ b/ConfigData/Xlsx/Bless.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="190">
   <si>
     <t>序列</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -749,6 +749,26 @@
   </si>
   <si>
     <t>Ename</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MoveSameCostFood</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>回头路消耗</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>moven2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>如果进入走过的格子，造成额外的食物消耗</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>彷徨</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1550,7 +1570,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1669,6 +1689,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="51" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="50" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1718,35 +1747,6 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="21">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1881,6 +1881,35 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -2063,6 +2092,72 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
     <mruColors>
       <color rgb="FFB31D96"/>
       <color rgb="FFF577AD"/>
@@ -2080,19 +2175,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AI37" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18" headerRowCellStyle="百分比">
-  <autoFilter ref="A3:AI37"/>
-  <tableColumns count="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AJ38" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18" headerRowCellStyle="百分比">
+  <autoFilter ref="A3:AJ38"/>
+  <sortState ref="A4:AJ38">
+    <sortCondition ref="A3:A38"/>
+  </sortState>
+  <tableColumns count="36">
     <tableColumn id="1" name="Id" dataDxfId="17"/>
     <tableColumn id="14" name="Type" dataDxfId="16"/>
     <tableColumn id="5" name="Level" dataDxfId="15"/>
     <tableColumn id="2" name="Name" dataDxfId="14"/>
-    <tableColumn id="35" name="Ename" dataDxfId="0"/>
-    <tableColumn id="3" name="Descript" dataDxfId="13"/>
+    <tableColumn id="35" name="Ename" dataDxfId="13"/>
+    <tableColumn id="3" name="Descript" dataDxfId="12"/>
     <tableColumn id="25" name="Round"/>
-    <tableColumn id="4" name="MoveFoodChange" dataDxfId="12"/>
+    <tableColumn id="4" name="MoveFoodChange" dataDxfId="11"/>
     <tableColumn id="20" name="MoveDistance"/>
     <tableColumn id="34" name="MoveCostHp"/>
+    <tableColumn id="36" name="MoveSameCostFood"/>
     <tableColumn id="8" name="RewardGoldMulti"/>
     <tableColumn id="7" name="RewardFoodMulti"/>
     <tableColumn id="6" name="RewardHealthMulti"/>
@@ -2106,7 +2205,7 @@
     <tableColumn id="17" name="RollWinAddGold"/>
     <tableColumn id="18" name="RollFailSubHealth"/>
     <tableColumn id="27" name="RollAlwaysWinBig"/>
-    <tableColumn id="26" name="RollAlwaysFailBig" dataDxfId="11"/>
+    <tableColumn id="26" name="RollAlwaysFailBig" dataDxfId="10"/>
     <tableColumn id="19" name="FightLevelChange"/>
     <tableColumn id="21" name="FightWinAddHealth"/>
     <tableColumn id="24" name="FightWinAddExp"/>
@@ -2117,7 +2216,7 @@
     <tableColumn id="31" name="TestAdjustPointTwo"/>
     <tableColumn id="32" name="TestBallChange"/>
     <tableColumn id="33" name="TestBallSynchonize"/>
-    <tableColumn id="9" name="Icon" dataDxfId="10"/>
+    <tableColumn id="9" name="Icon" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2131,7 +2230,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2444,10 +2543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI37"/>
+  <dimension ref="A1:AJ38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E37"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2457,15 +2556,15 @@
     <col min="5" max="5" width="6.375" customWidth="1"/>
     <col min="6" max="6" width="34.375" customWidth="1"/>
     <col min="7" max="7" width="4.875" customWidth="1"/>
-    <col min="8" max="10" width="4.5" customWidth="1"/>
-    <col min="11" max="22" width="3.875" customWidth="1"/>
-    <col min="23" max="24" width="4.5" customWidth="1"/>
-    <col min="25" max="33" width="3.875" customWidth="1"/>
-    <col min="34" max="34" width="4.625" customWidth="1"/>
-    <col min="38" max="38" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="4.5" customWidth="1"/>
+    <col min="12" max="23" width="3.875" customWidth="1"/>
+    <col min="24" max="25" width="4.5" customWidth="1"/>
+    <col min="26" max="34" width="3.875" customWidth="1"/>
+    <col min="35" max="35" width="4.625" customWidth="1"/>
+    <col min="39" max="39" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="66" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:36" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2496,83 +2595,86 @@
       <c r="J1" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="L1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="U1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="27" t="s">
+      <c r="V1" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="W1" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="W1" s="27" t="s">
+      <c r="X1" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="X1" s="27" t="s">
+      <c r="Y1" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="Y1" s="14" t="s">
+      <c r="Z1" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="AA1" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="AA1" s="14" t="s">
+      <c r="AB1" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="AB1" s="14" t="s">
+      <c r="AC1" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="AC1" s="14" t="s">
+      <c r="AD1" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="AD1" s="32" t="s">
+      <c r="AE1" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="AE1" s="32" t="s">
+      <c r="AF1" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="AF1" s="37" t="s">
+      <c r="AG1" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="AG1" s="37" t="s">
+      <c r="AH1" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="AH1" s="37" t="s">
+      <c r="AI1" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="AI1" s="10" t="s">
+      <c r="AJ1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2603,8 +2705,8 @@
       <c r="J2" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="K2" s="16" t="s">
-        <v>29</v>
+      <c r="K2" s="15" t="s">
+        <v>116</v>
       </c>
       <c r="L2" s="16" t="s">
         <v>29</v>
@@ -2619,10 +2721,10 @@
         <v>29</v>
       </c>
       <c r="P2" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" s="16" t="s">
         <v>128</v>
-      </c>
-      <c r="Q2" s="17" t="s">
-        <v>29</v>
       </c>
       <c r="R2" s="17" t="s">
         <v>29</v>
@@ -2633,20 +2735,20 @@
       <c r="T2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="U2" s="28" t="s">
+      <c r="U2" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="V2" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="V2" s="28" t="s">
+      <c r="W2" s="28" t="s">
         <v>66</v>
-      </c>
-      <c r="W2" s="28" t="s">
-        <v>116</v>
       </c>
       <c r="X2" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="Y2" s="18" t="s">
-        <v>75</v>
+      <c r="Y2" s="28" t="s">
+        <v>116</v>
       </c>
       <c r="Z2" s="18" t="s">
         <v>75</v>
@@ -2660,26 +2762,29 @@
       <c r="AC2" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="AD2" s="33" t="s">
-        <v>142</v>
+      <c r="AD2" s="18" t="s">
+        <v>75</v>
       </c>
       <c r="AE2" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="AF2" s="38" t="s">
-        <v>5</v>
+      <c r="AF2" s="33" t="s">
+        <v>142</v>
       </c>
       <c r="AG2" s="38" t="s">
         <v>5</v>
       </c>
       <c r="AH2" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI2" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -2710,83 +2815,86 @@
       <c r="J3" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="Q3" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="U3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="U3" s="29" t="s">
+      <c r="V3" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="V3" s="29" t="s">
+      <c r="W3" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="W3" s="29" t="s">
+      <c r="X3" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="X3" s="29" t="s">
+      <c r="Y3" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="Y3" s="7" t="s">
+      <c r="Z3" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="Z3" s="7" t="s">
+      <c r="AA3" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AA3" s="7" t="s">
+      <c r="AB3" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="AB3" s="7" t="s">
+      <c r="AC3" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="AC3" s="7" t="s">
+      <c r="AD3" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="AD3" s="34" t="s">
+      <c r="AE3" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="AE3" s="34" t="s">
+      <c r="AF3" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="AF3" s="39" t="s">
+      <c r="AG3" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="AG3" s="39" t="s">
+      <c r="AH3" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="AH3" s="39" t="s">
+      <c r="AI3" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="AI3" s="4" t="s">
+      <c r="AJ3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A4" s="23">
         <v>16000001</v>
       </c>
@@ -2811,12 +2919,12 @@
       <c r="H4">
         <v>-1</v>
       </c>
-      <c r="X4" s="26"/>
-      <c r="AI4" t="s">
+      <c r="Y4" s="26"/>
+      <c r="AJ4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A5" s="23">
         <v>16000002</v>
       </c>
@@ -2838,15 +2946,15 @@
       <c r="G5">
         <v>20</v>
       </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="X5" s="26"/>
-      <c r="AI5" t="s">
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="26"/>
+      <c r="AJ5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A6" s="23">
         <v>16000003</v>
       </c>
@@ -2868,15 +2976,15 @@
       <c r="G6">
         <v>20</v>
       </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="X6" s="26"/>
-      <c r="AI6" t="s">
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="26"/>
+      <c r="AJ6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A7" s="23">
         <v>16000004</v>
       </c>
@@ -2898,15 +3006,15 @@
       <c r="G7">
         <v>20</v>
       </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="X7" s="26"/>
-      <c r="AI7" t="s">
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="26"/>
+      <c r="AJ7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A8" s="23">
         <v>16000005</v>
       </c>
@@ -2928,15 +3036,15 @@
       <c r="G8">
         <v>20</v>
       </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
-      <c r="X8" s="26"/>
-      <c r="AI8" t="s">
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="26"/>
+      <c r="AJ8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A9" s="23">
         <v>16000006</v>
       </c>
@@ -2958,15 +3066,15 @@
       <c r="G9">
         <v>20</v>
       </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
-      <c r="X9" s="26"/>
-      <c r="AI9" t="s">
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="26"/>
+      <c r="AJ9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A10" s="23">
         <v>16000007</v>
       </c>
@@ -2988,15 +3096,15 @@
       <c r="G10">
         <v>20</v>
       </c>
-      <c r="V10">
-        <v>1</v>
-      </c>
-      <c r="X10" s="26"/>
-      <c r="AI10" t="s">
+      <c r="W10">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="26"/>
+      <c r="AJ10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A11" s="23">
         <v>16000008</v>
       </c>
@@ -3018,15 +3126,15 @@
       <c r="G11">
         <v>20</v>
       </c>
-      <c r="X11" s="26"/>
-      <c r="Z11">
-        <v>1</v>
-      </c>
-      <c r="AI11" s="35" t="s">
+      <c r="Y11" s="26"/>
+      <c r="AA11">
+        <v>1</v>
+      </c>
+      <c r="AJ11" s="35" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A12" s="23">
         <v>16000009</v>
       </c>
@@ -3051,12 +3159,12 @@
       <c r="I12">
         <v>1</v>
       </c>
-      <c r="X12" s="26"/>
-      <c r="AI12" s="36" t="s">
+      <c r="Y12" s="26"/>
+      <c r="AJ12" s="36" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A13" s="23">
         <v>16000010</v>
       </c>
@@ -3079,15 +3187,15 @@
         <v>20</v>
       </c>
       <c r="H13" s="30"/>
-      <c r="X13" s="26"/>
-      <c r="AD13" s="26" t="s">
+      <c r="Y13" s="26"/>
+      <c r="AE13" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="AI13" s="36" t="s">
+      <c r="AJ13" s="36" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A14" s="23">
         <v>16000011</v>
       </c>
@@ -3110,16 +3218,16 @@
         <v>20</v>
       </c>
       <c r="H14" s="22"/>
-      <c r="X14" s="26"/>
-      <c r="AD14" s="26"/>
-      <c r="AF14">
-        <v>1</v>
-      </c>
-      <c r="AI14" s="22" t="s">
+      <c r="Y14" s="26"/>
+      <c r="AE14" s="26"/>
+      <c r="AG14">
+        <v>1</v>
+      </c>
+      <c r="AJ14" s="22" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A15" s="23">
         <v>16001001</v>
       </c>
@@ -3141,18 +3249,18 @@
       <c r="G15">
         <v>20</v>
       </c>
-      <c r="X15" s="26"/>
-      <c r="Z15">
-        <v>1</v>
-      </c>
+      <c r="Y15" s="26"/>
       <c r="AA15">
         <v>1</v>
       </c>
-      <c r="AI15" s="35" t="s">
+      <c r="AB15">
+        <v>1</v>
+      </c>
+      <c r="AJ15" s="35" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A16" s="23">
         <v>16001002</v>
       </c>
@@ -3174,15 +3282,15 @@
       <c r="G16">
         <v>10</v>
       </c>
-      <c r="W16" s="26" t="s">
+      <c r="X16" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="X16" s="26"/>
-      <c r="AI16" s="35" t="s">
+      <c r="Y16" s="26"/>
+      <c r="AJ16" s="35" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A17" s="23">
         <v>16001003</v>
       </c>
@@ -3205,16 +3313,16 @@
         <v>20</v>
       </c>
       <c r="H17" s="30"/>
-      <c r="P17">
-        <v>1</v>
-      </c>
-      <c r="W17" s="26"/>
+      <c r="Q17">
+        <v>1</v>
+      </c>
       <c r="X17" s="26"/>
-      <c r="AI17" s="36" t="s">
+      <c r="Y17" s="26"/>
+      <c r="AJ17" s="36" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A18" s="23">
         <v>16001004</v>
       </c>
@@ -3237,16 +3345,16 @@
         <v>20</v>
       </c>
       <c r="H18" s="22"/>
-      <c r="W18" s="26"/>
       <c r="X18" s="26"/>
-      <c r="AG18">
-        <v>1</v>
-      </c>
-      <c r="AI18" s="22" t="s">
+      <c r="Y18" s="26"/>
+      <c r="AH18">
+        <v>1</v>
+      </c>
+      <c r="AJ18" s="22" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A19" s="23">
         <v>16002001</v>
       </c>
@@ -3269,9 +3377,6 @@
         <v>20</v>
       </c>
       <c r="H19" s="22"/>
-      <c r="K19">
-        <v>1</v>
-      </c>
       <c r="L19">
         <v>1</v>
       </c>
@@ -3281,12 +3386,15 @@
       <c r="N19">
         <v>1</v>
       </c>
-      <c r="X19" s="26"/>
-      <c r="AI19" s="35" t="s">
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="Y19" s="26"/>
+      <c r="AJ19" s="35" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A20" s="23">
         <v>16002002</v>
       </c>
@@ -3311,12 +3419,12 @@
       <c r="I20">
         <v>98</v>
       </c>
-      <c r="X20" s="26"/>
-      <c r="AI20" s="36" t="s">
+      <c r="Y20" s="26"/>
+      <c r="AJ20" s="36" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A21" s="24">
         <v>16010001</v>
       </c>
@@ -3341,12 +3449,12 @@
       <c r="H21">
         <v>1</v>
       </c>
-      <c r="X21" s="26"/>
-      <c r="AI21" s="35" t="s">
+      <c r="Y21" s="26"/>
+      <c r="AJ21" s="35" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A22" s="24">
         <v>16010002</v>
       </c>
@@ -3368,15 +3476,15 @@
       <c r="G22">
         <v>20</v>
       </c>
-      <c r="Q22">
-        <v>1</v>
-      </c>
-      <c r="X22" s="26"/>
-      <c r="AI22" s="35" t="s">
+      <c r="R22">
+        <v>1</v>
+      </c>
+      <c r="Y22" s="26"/>
+      <c r="AJ22" s="35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A23" s="24">
         <v>16010003</v>
       </c>
@@ -3398,15 +3506,15 @@
       <c r="G23">
         <v>20</v>
       </c>
-      <c r="R23">
-        <v>1</v>
-      </c>
-      <c r="X23" s="26"/>
-      <c r="AI23" s="35" t="s">
+      <c r="S23">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="26"/>
+      <c r="AJ23" s="35" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A24" s="24">
         <v>16010004</v>
       </c>
@@ -3428,15 +3536,15 @@
       <c r="G24">
         <v>20</v>
       </c>
-      <c r="S24">
-        <v>1</v>
-      </c>
-      <c r="X24" s="26"/>
-      <c r="AI24" s="35" t="s">
+      <c r="T24">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="26"/>
+      <c r="AJ24" s="35" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A25" s="24">
         <v>16010005</v>
       </c>
@@ -3458,15 +3566,15 @@
       <c r="G25">
         <v>20</v>
       </c>
-      <c r="T25">
-        <v>1</v>
-      </c>
-      <c r="X25" s="26"/>
-      <c r="AI25" s="35" t="s">
+      <c r="U25">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="26"/>
+      <c r="AJ25" s="35" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A26" s="24">
         <v>16010006</v>
       </c>
@@ -3488,15 +3596,15 @@
       <c r="G26">
         <v>20</v>
       </c>
-      <c r="O26">
+      <c r="P26">
         <v>-1</v>
       </c>
-      <c r="X26" s="26"/>
-      <c r="AI26" s="35" t="s">
+      <c r="Y26" s="26"/>
+      <c r="AJ26" s="35" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A27" s="24">
         <v>16010007</v>
       </c>
@@ -3518,15 +3626,15 @@
       <c r="G27">
         <v>20</v>
       </c>
-      <c r="U27">
-        <v>1</v>
-      </c>
-      <c r="X27" s="26"/>
-      <c r="AI27" s="35" t="s">
+      <c r="V27">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="26"/>
+      <c r="AJ27" s="35" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A28" s="24">
         <v>16010008</v>
       </c>
@@ -3548,15 +3656,15 @@
       <c r="G28">
         <v>20</v>
       </c>
-      <c r="X28" s="26"/>
-      <c r="AB28">
-        <v>1</v>
-      </c>
-      <c r="AI28" s="35" t="s">
+      <c r="Y28" s="26"/>
+      <c r="AC28">
+        <v>1</v>
+      </c>
+      <c r="AJ28" s="35" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A29" s="24">
         <v>16010009</v>
       </c>
@@ -3579,15 +3687,15 @@
         <v>20</v>
       </c>
       <c r="H29" s="22"/>
-      <c r="X29" s="26"/>
-      <c r="AD29">
+      <c r="Y29" s="26"/>
+      <c r="AE29">
         <v>0.5</v>
       </c>
-      <c r="AI29" s="35" t="s">
+      <c r="AJ29" s="35" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A30" s="24">
         <v>16010010</v>
       </c>
@@ -3610,15 +3718,15 @@
         <v>20</v>
       </c>
       <c r="H30" s="22"/>
-      <c r="X30" s="26"/>
-      <c r="AF30">
+      <c r="Y30" s="26"/>
+      <c r="AG30">
         <v>-1</v>
       </c>
-      <c r="AI30" s="22" t="s">
+      <c r="AJ30" s="22" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A31" s="24">
         <v>16010011</v>
       </c>
@@ -3641,15 +3749,15 @@
         <v>20</v>
       </c>
       <c r="H31" s="22"/>
-      <c r="X31" s="26"/>
-      <c r="AH31" s="26" t="s">
+      <c r="Y31" s="26"/>
+      <c r="AI31" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="AI31" s="22" t="s">
+      <c r="AJ31" s="22" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A32" s="24">
         <v>16011001</v>
       </c>
@@ -3671,18 +3779,18 @@
       <c r="G32">
         <v>20</v>
       </c>
-      <c r="X32" s="26"/>
-      <c r="AB32">
-        <v>1</v>
-      </c>
+      <c r="Y32" s="26"/>
       <c r="AC32">
         <v>1</v>
       </c>
-      <c r="AI32" s="35" t="s">
+      <c r="AD32">
+        <v>1</v>
+      </c>
+      <c r="AJ32" s="35" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A33" s="24">
         <v>16011002</v>
       </c>
@@ -3705,14 +3813,14 @@
         <v>10</v>
       </c>
       <c r="H33" s="22"/>
-      <c r="X33" s="26" t="s">
+      <c r="Y33" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="AI33" t="s">
+      <c r="AJ33" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A34" s="24">
         <v>16011003</v>
       </c>
@@ -3735,56 +3843,49 @@
         <v>20</v>
       </c>
       <c r="H34" s="22"/>
-      <c r="X34" s="26"/>
-      <c r="AG34">
+      <c r="Y34" s="26"/>
+      <c r="AH34">
         <v>-1</v>
       </c>
-      <c r="AI34" s="22" t="s">
+      <c r="AJ34" s="22" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A35" s="24">
-        <v>16012001</v>
+        <v>16011004</v>
       </c>
       <c r="B35">
         <v>2</v>
       </c>
       <c r="C35">
-        <v>3</v>
-      </c>
-      <c r="D35" t="s">
-        <v>100</v>
-      </c>
-      <c r="E35" t="s">
-        <v>98</v>
-      </c>
-      <c r="F35" t="s">
-        <v>154</v>
+        <v>2</v>
+      </c>
+      <c r="D35" s="41" t="s">
+        <v>189</v>
+      </c>
+      <c r="E35" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="F35" s="41" t="s">
+        <v>188</v>
       </c>
       <c r="G35">
         <v>20</v>
       </c>
-      <c r="Q35">
-        <v>1</v>
-      </c>
-      <c r="R35">
-        <v>1</v>
-      </c>
-      <c r="S35">
-        <v>1</v>
-      </c>
-      <c r="T35">
-        <v>1</v>
-      </c>
-      <c r="X35" s="26"/>
-      <c r="AI35" t="s">
-        <v>98</v>
+      <c r="H35" s="41"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y35" s="26"/>
+      <c r="AJ35" s="42" t="s">
+        <v>181</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A36" s="24">
-        <v>16012002</v>
+        <v>16012001</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -3792,103 +3893,144 @@
       <c r="C36">
         <v>3</v>
       </c>
-      <c r="D36" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="E36" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="F36" s="22" t="s">
-        <v>180</v>
+      <c r="D36" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="E36" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="F36" s="40" t="s">
+        <v>154</v>
       </c>
       <c r="G36">
         <v>20</v>
       </c>
-      <c r="H36" s="22"/>
-      <c r="J36" s="26" t="s">
+      <c r="H36" s="40"/>
+      <c r="R36">
+        <v>1</v>
+      </c>
+      <c r="S36">
+        <v>1</v>
+      </c>
+      <c r="T36">
+        <v>1</v>
+      </c>
+      <c r="U36">
+        <v>1</v>
+      </c>
+      <c r="Y36" s="26"/>
+      <c r="AJ36" s="40" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:36" x14ac:dyDescent="0.15">
+      <c r="A37" s="24">
+        <v>16012002</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="F37" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="G37">
+        <v>20</v>
+      </c>
+      <c r="H37" s="22"/>
+      <c r="J37" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="X36" s="26"/>
-      <c r="AI36" s="22" t="s">
+      <c r="K37" s="26"/>
+      <c r="Y37" s="26"/>
+      <c r="AJ37" s="22" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.15">
-      <c r="A37" s="25">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.15">
+      <c r="A38" s="25">
         <v>16020001</v>
       </c>
-      <c r="B37" s="22">
+      <c r="B38" s="22">
         <v>3</v>
       </c>
-      <c r="C37" s="22">
-        <v>1</v>
-      </c>
-      <c r="D37" s="22" t="s">
+      <c r="C38" s="22">
+        <v>1</v>
+      </c>
+      <c r="D38" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="E37" s="22" t="s">
+      <c r="E38" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F38" t="s">
         <v>109</v>
       </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
-      <c r="H37" s="22"/>
-      <c r="I37">
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38" s="22"/>
+      <c r="I38">
         <v>98</v>
       </c>
-      <c r="X37" s="26"/>
-      <c r="AI37" s="22" t="s">
+      <c r="Y38" s="26"/>
+      <c r="AJ38" s="22" t="s">
         <v>111</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B30:D30 B4:D17 B19:D28 H18:AI18 H34:AI34 B32:D33 H29:AI31 B35:D37 F35:AI37 F32:AI33 F19:AI28 F4:AI17 F30:G30">
-    <cfRule type="containsBlanks" dxfId="9" priority="14">
+  <conditionalFormatting sqref="B30:D30 B4:D17 B19:D28 H18:AJ18 H34:AJ34 B32:D33 H29:AJ31 F32:AJ33 F19:AJ28 F4:AJ17 F30:G30 B35:D36 E4:E36 B38:AJ38 F35:AJ36">
+    <cfRule type="containsBlanks" dxfId="8" priority="15">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:D29 G29">
-    <cfRule type="containsBlanks" dxfId="8" priority="8">
+    <cfRule type="containsBlanks" dxfId="7" priority="9">
       <formula>LEN(TRIM(B29))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29">
-    <cfRule type="containsBlanks" dxfId="7" priority="7">
+    <cfRule type="containsBlanks" dxfId="6" priority="8">
       <formula>LEN(TRIM(F29))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:D18 G18">
-    <cfRule type="containsBlanks" dxfId="6" priority="6">
+    <cfRule type="containsBlanks" dxfId="5" priority="7">
       <formula>LEN(TRIM(B18))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="containsBlanks" dxfId="5" priority="5">
+    <cfRule type="containsBlanks" dxfId="4" priority="6">
       <formula>LEN(TRIM(F18))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34:D34 G34">
-    <cfRule type="containsBlanks" dxfId="4" priority="4">
+    <cfRule type="containsBlanks" dxfId="3" priority="5">
       <formula>LEN(TRIM(B34))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34">
-    <cfRule type="containsBlanks" dxfId="3" priority="3">
+    <cfRule type="containsBlanks" dxfId="2" priority="4">
       <formula>LEN(TRIM(F34))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31:D31 F31:G31">
-    <cfRule type="containsBlanks" dxfId="2" priority="2">
+    <cfRule type="containsBlanks" dxfId="1" priority="3">
       <formula>LEN(TRIM(B31))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4:E37">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
-      <formula>LEN(TRIM(E4))=0</formula>
+  <conditionalFormatting sqref="B37:AJ37">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(B37))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add a newbie bless for new player
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Bless.xlsx
+++ b/ConfigData/Xlsx/Bless.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="198">
   <si>
     <t>序列</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -756,10 +756,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>回头路消耗</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>moven2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -769,6 +765,41 @@
   </si>
   <si>
     <t>彷徨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsRandom</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>newbie</t>
+  </si>
+  <si>
+    <t>newbie</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>新手保护</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>回头路消耗增加</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>移动消耗食物-1，战斗时己方卡牌等级+1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1746,7 +1777,24 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2092,72 +2140,6 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
     <mruColors>
       <color rgb="FFB31D96"/>
       <color rgb="FFF577AD"/>
@@ -2175,20 +2157,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AJ38" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18" headerRowCellStyle="百分比">
-  <autoFilter ref="A3:AJ38"/>
-  <sortState ref="A4:AJ38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AK39" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21" headerRowCellStyle="百分比">
+  <autoFilter ref="A3:AK39"/>
+  <sortState ref="A4:AK38">
     <sortCondition ref="A3:A38"/>
   </sortState>
-  <tableColumns count="36">
-    <tableColumn id="1" name="Id" dataDxfId="17"/>
-    <tableColumn id="14" name="Type" dataDxfId="16"/>
-    <tableColumn id="5" name="Level" dataDxfId="15"/>
-    <tableColumn id="2" name="Name" dataDxfId="14"/>
-    <tableColumn id="35" name="Ename" dataDxfId="13"/>
-    <tableColumn id="3" name="Descript" dataDxfId="12"/>
+  <tableColumns count="37">
+    <tableColumn id="1" name="Id" dataDxfId="20"/>
+    <tableColumn id="14" name="Type" dataDxfId="19"/>
+    <tableColumn id="5" name="Level" dataDxfId="18"/>
+    <tableColumn id="2" name="Name" dataDxfId="17"/>
+    <tableColumn id="35" name="Ename" dataDxfId="16"/>
+    <tableColumn id="3" name="Descript" dataDxfId="15"/>
+    <tableColumn id="37" name="IsRandom" dataDxfId="2"/>
     <tableColumn id="25" name="Round"/>
-    <tableColumn id="4" name="MoveFoodChange" dataDxfId="11"/>
+    <tableColumn id="4" name="MoveFoodChange" dataDxfId="14"/>
     <tableColumn id="20" name="MoveDistance"/>
     <tableColumn id="34" name="MoveCostHp"/>
     <tableColumn id="36" name="MoveSameCostFood"/>
@@ -2205,7 +2188,7 @@
     <tableColumn id="17" name="RollWinAddGold"/>
     <tableColumn id="18" name="RollFailSubHealth"/>
     <tableColumn id="27" name="RollAlwaysWinBig"/>
-    <tableColumn id="26" name="RollAlwaysFailBig" dataDxfId="10"/>
+    <tableColumn id="26" name="RollAlwaysFailBig" dataDxfId="13"/>
     <tableColumn id="19" name="FightLevelChange"/>
     <tableColumn id="21" name="FightWinAddHealth"/>
     <tableColumn id="24" name="FightWinAddExp"/>
@@ -2216,7 +2199,7 @@
     <tableColumn id="31" name="TestAdjustPointTwo"/>
     <tableColumn id="32" name="TestBallChange"/>
     <tableColumn id="33" name="TestBallSynchonize"/>
-    <tableColumn id="9" name="Icon" dataDxfId="9"/>
+    <tableColumn id="9" name="Icon" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2230,7 +2213,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2543,28 +2526,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ38"/>
+  <dimension ref="A1:AK39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="G25" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="AK39" sqref="AK39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="5.125" customWidth="1"/>
-    <col min="5" max="5" width="6.375" customWidth="1"/>
+    <col min="2" max="3" width="3.5" customWidth="1"/>
+    <col min="4" max="4" width="7.875" customWidth="1"/>
+    <col min="5" max="5" width="8.125" customWidth="1"/>
     <col min="6" max="6" width="34.375" customWidth="1"/>
-    <col min="7" max="7" width="4.875" customWidth="1"/>
-    <col min="8" max="11" width="4.5" customWidth="1"/>
-    <col min="12" max="23" width="3.875" customWidth="1"/>
-    <col min="24" max="25" width="4.5" customWidth="1"/>
-    <col min="26" max="34" width="3.875" customWidth="1"/>
-    <col min="35" max="35" width="4.625" customWidth="1"/>
-    <col min="39" max="39" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.75" customWidth="1"/>
+    <col min="8" max="8" width="4.875" customWidth="1"/>
+    <col min="9" max="12" width="4.5" customWidth="1"/>
+    <col min="13" max="24" width="3.875" customWidth="1"/>
+    <col min="25" max="26" width="4.5" customWidth="1"/>
+    <col min="27" max="35" width="3.875" customWidth="1"/>
+    <col min="36" max="36" width="4.625" customWidth="1"/>
+    <col min="40" max="40" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="66" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:37" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2583,98 +2571,101 @@
       <c r="F1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="H1" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="K1" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="M1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="U1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="V1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="W1" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="W1" s="27" t="s">
+      <c r="X1" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="X1" s="27" t="s">
+      <c r="Y1" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="Y1" s="27" t="s">
+      <c r="Z1" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="AA1" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="AA1" s="14" t="s">
+      <c r="AB1" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="AB1" s="14" t="s">
+      <c r="AC1" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="AC1" s="14" t="s">
+      <c r="AD1" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="AD1" s="14" t="s">
+      <c r="AE1" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="AE1" s="32" t="s">
+      <c r="AF1" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="AF1" s="32" t="s">
+      <c r="AG1" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="AG1" s="37" t="s">
+      <c r="AH1" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="AH1" s="37" t="s">
+      <c r="AI1" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="AI1" s="37" t="s">
+      <c r="AJ1" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="AJ1" s="10" t="s">
+      <c r="AK1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2693,23 +2684,23 @@
       <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="H2" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="J2" s="15" t="s">
         <v>29</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>116</v>
       </c>
       <c r="K2" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="L2" s="16" t="s">
-        <v>29</v>
+      <c r="L2" s="15" t="s">
+        <v>116</v>
       </c>
       <c r="M2" s="16" t="s">
         <v>29</v>
@@ -2724,10 +2715,10 @@
         <v>29</v>
       </c>
       <c r="Q2" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2" s="16" t="s">
         <v>128</v>
-      </c>
-      <c r="R2" s="17" t="s">
-        <v>29</v>
       </c>
       <c r="S2" s="17" t="s">
         <v>29</v>
@@ -2738,20 +2729,20 @@
       <c r="U2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="V2" s="28" t="s">
+      <c r="V2" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="W2" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="W2" s="28" t="s">
+      <c r="X2" s="28" t="s">
         <v>66</v>
-      </c>
-      <c r="X2" s="28" t="s">
-        <v>116</v>
       </c>
       <c r="Y2" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="Z2" s="18" t="s">
-        <v>75</v>
+      <c r="Z2" s="28" t="s">
+        <v>116</v>
       </c>
       <c r="AA2" s="18" t="s">
         <v>75</v>
@@ -2765,26 +2756,29 @@
       <c r="AD2" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="AE2" s="33" t="s">
-        <v>142</v>
+      <c r="AE2" s="18" t="s">
+        <v>75</v>
       </c>
       <c r="AF2" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="AG2" s="38" t="s">
-        <v>5</v>
+      <c r="AG2" s="33" t="s">
+        <v>142</v>
       </c>
       <c r="AH2" s="38" t="s">
         <v>5</v>
       </c>
       <c r="AI2" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ2" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AK2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -2803,98 +2797,101 @@
       <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="H3" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="Q3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="R3" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="U3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="V3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="V3" s="29" t="s">
+      <c r="W3" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="W3" s="29" t="s">
+      <c r="X3" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="X3" s="29" t="s">
+      <c r="Y3" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="Y3" s="29" t="s">
+      <c r="Z3" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="Z3" s="7" t="s">
+      <c r="AA3" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="AA3" s="7" t="s">
+      <c r="AB3" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AB3" s="7" t="s">
+      <c r="AC3" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="AC3" s="7" t="s">
+      <c r="AD3" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="AD3" s="7" t="s">
+      <c r="AE3" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="AE3" s="34" t="s">
+      <c r="AF3" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="AF3" s="34" t="s">
+      <c r="AG3" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="AG3" s="39" t="s">
+      <c r="AH3" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="AH3" s="39" t="s">
+      <c r="AI3" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="AI3" s="39" t="s">
+      <c r="AJ3" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="AJ3" s="4" t="s">
+      <c r="AK3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A4" s="23">
         <v>16000001</v>
       </c>
@@ -2913,18 +2910,21 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H4">
         <v>20</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>-1</v>
       </c>
-      <c r="Y4" s="26"/>
-      <c r="AJ4" t="s">
+      <c r="Z4" s="26"/>
+      <c r="AK4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A5" s="23">
         <v>16000002</v>
       </c>
@@ -2943,18 +2943,21 @@
       <c r="F5" t="s">
         <v>145</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H5">
         <v>20</v>
       </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="26"/>
-      <c r="AJ5" t="s">
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="26"/>
+      <c r="AK5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A6" s="23">
         <v>16000003</v>
       </c>
@@ -2973,18 +2976,21 @@
       <c r="F6" t="s">
         <v>146</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H6">
         <v>20</v>
       </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="26"/>
-      <c r="AJ6" t="s">
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="26"/>
+      <c r="AK6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A7" s="23">
         <v>16000004</v>
       </c>
@@ -3003,18 +3009,21 @@
       <c r="F7" t="s">
         <v>147</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H7">
         <v>20</v>
       </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="26"/>
-      <c r="AJ7" t="s">
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="26"/>
+      <c r="AK7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A8" s="23">
         <v>16000005</v>
       </c>
@@ -3033,18 +3042,21 @@
       <c r="F8" t="s">
         <v>148</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H8">
         <v>20</v>
       </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="26"/>
-      <c r="AJ8" t="s">
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="26"/>
+      <c r="AK8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A9" s="23">
         <v>16000006</v>
       </c>
@@ -3063,18 +3075,21 @@
       <c r="F9" t="s">
         <v>149</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H9">
         <v>20</v>
       </c>
-      <c r="P9">
-        <v>1</v>
-      </c>
-      <c r="Y9" s="26"/>
-      <c r="AJ9" t="s">
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="26"/>
+      <c r="AK9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A10" s="23">
         <v>16000007</v>
       </c>
@@ -3093,18 +3108,21 @@
       <c r="F10" t="s">
         <v>114</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H10">
         <v>20</v>
       </c>
-      <c r="W10">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="26"/>
-      <c r="AJ10" t="s">
+      <c r="X10">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="26"/>
+      <c r="AK10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A11" s="23">
         <v>16000008</v>
       </c>
@@ -3123,18 +3141,21 @@
       <c r="F11" t="s">
         <v>88</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H11">
         <v>20</v>
       </c>
-      <c r="Y11" s="26"/>
-      <c r="AA11">
-        <v>1</v>
-      </c>
-      <c r="AJ11" s="35" t="s">
+      <c r="Z11" s="26"/>
+      <c r="AB11">
+        <v>1</v>
+      </c>
+      <c r="AK11" s="35" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A12" s="23">
         <v>16000009</v>
       </c>
@@ -3153,18 +3174,21 @@
       <c r="F12" t="s">
         <v>107</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H12">
         <v>10</v>
       </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="Y12" s="26"/>
-      <c r="AJ12" s="36" t="s">
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="26"/>
+      <c r="AK12" s="36" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A13" s="23">
         <v>16000010</v>
       </c>
@@ -3183,19 +3207,22 @@
       <c r="F13" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H13">
         <v>20</v>
       </c>
-      <c r="H13" s="30"/>
-      <c r="Y13" s="26"/>
-      <c r="AE13" s="26" t="s">
+      <c r="I13" s="30"/>
+      <c r="Z13" s="26"/>
+      <c r="AF13" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="AJ13" s="36" t="s">
+      <c r="AK13" s="36" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A14" s="23">
         <v>16000011</v>
       </c>
@@ -3214,20 +3241,23 @@
       <c r="F14" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H14">
         <v>20</v>
       </c>
-      <c r="H14" s="22"/>
-      <c r="Y14" s="26"/>
-      <c r="AE14" s="26"/>
-      <c r="AG14">
-        <v>1</v>
-      </c>
-      <c r="AJ14" s="22" t="s">
+      <c r="I14" s="22"/>
+      <c r="Z14" s="26"/>
+      <c r="AF14" s="26"/>
+      <c r="AH14">
+        <v>1</v>
+      </c>
+      <c r="AK14" s="22" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A15" s="23">
         <v>16001001</v>
       </c>
@@ -3246,21 +3276,24 @@
       <c r="F15" t="s">
         <v>92</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H15">
         <v>20</v>
       </c>
-      <c r="Y15" s="26"/>
-      <c r="AA15">
-        <v>1</v>
-      </c>
+      <c r="Z15" s="26"/>
       <c r="AB15">
         <v>1</v>
       </c>
-      <c r="AJ15" s="35" t="s">
+      <c r="AC15">
+        <v>1</v>
+      </c>
+      <c r="AK15" s="35" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A16" s="23">
         <v>16001002</v>
       </c>
@@ -3279,18 +3312,21 @@
       <c r="F16" t="s">
         <v>124</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H16">
         <v>10</v>
       </c>
-      <c r="X16" s="26" t="s">
+      <c r="Y16" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="Y16" s="26"/>
-      <c r="AJ16" s="35" t="s">
+      <c r="Z16" s="26"/>
+      <c r="AK16" s="35" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A17" s="23">
         <v>16001003</v>
       </c>
@@ -3309,20 +3345,23 @@
       <c r="F17" t="s">
         <v>131</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H17">
         <v>20</v>
       </c>
-      <c r="H17" s="30"/>
-      <c r="Q17">
-        <v>1</v>
-      </c>
-      <c r="X17" s="26"/>
+      <c r="I17" s="30"/>
+      <c r="R17">
+        <v>1</v>
+      </c>
       <c r="Y17" s="26"/>
-      <c r="AJ17" s="36" t="s">
+      <c r="Z17" s="26"/>
+      <c r="AK17" s="36" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A18" s="23">
         <v>16001004</v>
       </c>
@@ -3341,20 +3380,23 @@
       <c r="F18" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H18">
         <v>20</v>
       </c>
-      <c r="H18" s="22"/>
-      <c r="X18" s="26"/>
+      <c r="I18" s="22"/>
       <c r="Y18" s="26"/>
-      <c r="AH18">
-        <v>1</v>
-      </c>
-      <c r="AJ18" s="22" t="s">
+      <c r="Z18" s="26"/>
+      <c r="AI18">
+        <v>1</v>
+      </c>
+      <c r="AK18" s="22" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A19" s="23">
         <v>16002001</v>
       </c>
@@ -3373,13 +3415,13 @@
       <c r="F19" t="s">
         <v>155</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H19">
         <v>20</v>
       </c>
-      <c r="H19" s="22"/>
-      <c r="L19">
-        <v>1</v>
-      </c>
+      <c r="I19" s="22"/>
       <c r="M19">
         <v>1</v>
       </c>
@@ -3389,12 +3431,15 @@
       <c r="O19">
         <v>1</v>
       </c>
-      <c r="Y19" s="26"/>
-      <c r="AJ19" s="35" t="s">
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Z19" s="26"/>
+      <c r="AK19" s="35" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A20" s="23">
         <v>16002002</v>
       </c>
@@ -3413,18 +3458,21 @@
       <c r="F20" t="s">
         <v>109</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H20">
         <v>10</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>98</v>
       </c>
-      <c r="Y20" s="26"/>
-      <c r="AJ20" s="36" t="s">
+      <c r="Z20" s="26"/>
+      <c r="AK20" s="36" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A21" s="24">
         <v>16010001</v>
       </c>
@@ -3443,18 +3491,21 @@
       <c r="F21" t="s">
         <v>18</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H21">
         <v>20</v>
       </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="Y21" s="26"/>
-      <c r="AJ21" s="35" t="s">
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="Z21" s="26"/>
+      <c r="AK21" s="35" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A22" s="24">
         <v>16010002</v>
       </c>
@@ -3473,18 +3524,21 @@
       <c r="F22" t="s">
         <v>150</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H22">
         <v>20</v>
       </c>
-      <c r="R22">
-        <v>1</v>
-      </c>
-      <c r="Y22" s="26"/>
-      <c r="AJ22" s="35" t="s">
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="Z22" s="26"/>
+      <c r="AK22" s="35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A23" s="24">
         <v>16010003</v>
       </c>
@@ -3503,18 +3557,21 @@
       <c r="F23" t="s">
         <v>151</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H23">
         <v>20</v>
       </c>
-      <c r="S23">
-        <v>1</v>
-      </c>
-      <c r="Y23" s="26"/>
-      <c r="AJ23" s="35" t="s">
+      <c r="T23">
+        <v>1</v>
+      </c>
+      <c r="Z23" s="26"/>
+      <c r="AK23" s="35" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A24" s="24">
         <v>16010004</v>
       </c>
@@ -3533,18 +3590,21 @@
       <c r="F24" t="s">
         <v>152</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H24">
         <v>20</v>
       </c>
-      <c r="T24">
-        <v>1</v>
-      </c>
-      <c r="Y24" s="26"/>
-      <c r="AJ24" s="35" t="s">
+      <c r="U24">
+        <v>1</v>
+      </c>
+      <c r="Z24" s="26"/>
+      <c r="AK24" s="35" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A25" s="24">
         <v>16010005</v>
       </c>
@@ -3563,18 +3623,21 @@
       <c r="F25" t="s">
         <v>153</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H25">
         <v>20</v>
       </c>
-      <c r="U25">
-        <v>1</v>
-      </c>
-      <c r="Y25" s="26"/>
-      <c r="AJ25" s="35" t="s">
+      <c r="V25">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="26"/>
+      <c r="AK25" s="35" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A26" s="24">
         <v>16010006</v>
       </c>
@@ -3593,18 +3656,21 @@
       <c r="F26" t="s">
         <v>63</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H26">
         <v>20</v>
       </c>
-      <c r="P26">
+      <c r="Q26">
         <v>-1</v>
       </c>
-      <c r="Y26" s="26"/>
-      <c r="AJ26" s="35" t="s">
+      <c r="Z26" s="26"/>
+      <c r="AK26" s="35" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A27" s="24">
         <v>16010007</v>
       </c>
@@ -3623,18 +3689,21 @@
       <c r="F27" t="s">
         <v>113</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H27">
         <v>20</v>
       </c>
-      <c r="V27">
-        <v>1</v>
-      </c>
-      <c r="Y27" s="26"/>
-      <c r="AJ27" s="35" t="s">
+      <c r="W27">
+        <v>1</v>
+      </c>
+      <c r="Z27" s="26"/>
+      <c r="AK27" s="35" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A28" s="24">
         <v>16010008</v>
       </c>
@@ -3653,18 +3722,21 @@
       <c r="F28" t="s">
         <v>90</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H28">
         <v>20</v>
       </c>
-      <c r="Y28" s="26"/>
-      <c r="AC28">
-        <v>1</v>
-      </c>
-      <c r="AJ28" s="35" t="s">
+      <c r="Z28" s="26"/>
+      <c r="AD28">
+        <v>1</v>
+      </c>
+      <c r="AK28" s="35" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A29" s="24">
         <v>16010009</v>
       </c>
@@ -3683,19 +3755,22 @@
       <c r="F29" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H29">
         <v>20</v>
       </c>
-      <c r="H29" s="22"/>
-      <c r="Y29" s="26"/>
-      <c r="AE29">
+      <c r="I29" s="22"/>
+      <c r="Z29" s="26"/>
+      <c r="AF29">
         <v>0.5</v>
       </c>
-      <c r="AJ29" s="35" t="s">
+      <c r="AK29" s="35" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A30" s="24">
         <v>16010010</v>
       </c>
@@ -3714,19 +3789,22 @@
       <c r="F30" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H30">
         <v>20</v>
       </c>
-      <c r="H30" s="22"/>
-      <c r="Y30" s="26"/>
-      <c r="AG30">
+      <c r="I30" s="22"/>
+      <c r="Z30" s="26"/>
+      <c r="AH30">
         <v>-1</v>
       </c>
-      <c r="AJ30" s="22" t="s">
+      <c r="AK30" s="22" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A31" s="24">
         <v>16010011</v>
       </c>
@@ -3745,19 +3823,22 @@
       <c r="F31" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H31">
         <v>20</v>
       </c>
-      <c r="H31" s="22"/>
-      <c r="Y31" s="26"/>
-      <c r="AI31" s="26" t="s">
+      <c r="I31" s="22"/>
+      <c r="Z31" s="26"/>
+      <c r="AJ31" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="AJ31" s="22" t="s">
+      <c r="AK31" s="22" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A32" s="24">
         <v>16011001</v>
       </c>
@@ -3776,21 +3857,24 @@
       <c r="F32" t="s">
         <v>95</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H32">
         <v>20</v>
       </c>
-      <c r="Y32" s="26"/>
-      <c r="AC32">
-        <v>1</v>
-      </c>
+      <c r="Z32" s="26"/>
       <c r="AD32">
         <v>1</v>
       </c>
-      <c r="AJ32" s="35" t="s">
+      <c r="AE32">
+        <v>1</v>
+      </c>
+      <c r="AK32" s="35" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A33" s="24">
         <v>16011002</v>
       </c>
@@ -3809,18 +3893,21 @@
       <c r="F33" t="s">
         <v>118</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H33">
         <v>10</v>
       </c>
-      <c r="H33" s="22"/>
-      <c r="Y33" s="26" t="s">
+      <c r="I33" s="22"/>
+      <c r="Z33" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="AJ33" t="s">
+      <c r="AK33" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A34" s="24">
         <v>16011003</v>
       </c>
@@ -3839,19 +3926,22 @@
       <c r="F34" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H34">
         <v>20</v>
       </c>
-      <c r="H34" s="22"/>
-      <c r="Y34" s="26"/>
-      <c r="AH34">
+      <c r="I34" s="22"/>
+      <c r="Z34" s="26"/>
+      <c r="AI34">
         <v>-1</v>
       </c>
-      <c r="AJ34" s="22" t="s">
+      <c r="AK34" s="22" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A35" s="24">
         <v>16011004</v>
       </c>
@@ -3862,28 +3952,31 @@
         <v>2</v>
       </c>
       <c r="D35" s="41" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E35" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="F35" s="41" t="s">
         <v>187</v>
       </c>
-      <c r="F35" s="41" t="s">
-        <v>188</v>
-      </c>
-      <c r="G35">
+      <c r="G35" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H35">
         <v>20</v>
       </c>
-      <c r="H35" s="41"/>
-      <c r="J35" s="26"/>
-      <c r="K35" s="26" t="s">
+      <c r="I35" s="41"/>
+      <c r="K35" s="26"/>
+      <c r="L35" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="Y35" s="26"/>
-      <c r="AJ35" s="42" t="s">
+      <c r="Z35" s="26"/>
+      <c r="AK35" s="42" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A36" s="24">
         <v>16012001</v>
       </c>
@@ -3902,13 +3995,13 @@
       <c r="F36" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H36">
         <v>20</v>
       </c>
-      <c r="H36" s="40"/>
-      <c r="R36">
-        <v>1</v>
-      </c>
+      <c r="I36" s="40"/>
       <c r="S36">
         <v>1</v>
       </c>
@@ -3918,12 +4011,15 @@
       <c r="U36">
         <v>1</v>
       </c>
-      <c r="Y36" s="26"/>
-      <c r="AJ36" s="40" t="s">
+      <c r="V36">
+        <v>1</v>
+      </c>
+      <c r="Z36" s="26"/>
+      <c r="AK36" s="40" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A37" s="24">
         <v>16012002</v>
       </c>
@@ -3942,20 +4038,23 @@
       <c r="F37" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H37">
         <v>20</v>
       </c>
-      <c r="H37" s="22"/>
-      <c r="J37" s="26" t="s">
+      <c r="I37" s="22"/>
+      <c r="K37" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="K37" s="26"/>
-      <c r="Y37" s="26"/>
-      <c r="AJ37" s="22" t="s">
+      <c r="L37" s="26"/>
+      <c r="Z37" s="26"/>
+      <c r="AK37" s="22" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A38" s="25">
         <v>16020001</v>
       </c>
@@ -3974,63 +4073,108 @@
       <c r="F38" t="s">
         <v>109</v>
       </c>
-      <c r="G38">
-        <v>1</v>
-      </c>
-      <c r="H38" s="22"/>
-      <c r="I38">
+      <c r="G38" s="26"/>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38" s="22"/>
+      <c r="J38">
         <v>98</v>
       </c>
-      <c r="Y38" s="26"/>
-      <c r="AJ38" s="22" t="s">
+      <c r="Z38" s="26"/>
+      <c r="AK38" s="22" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A39" s="25">
+        <v>16020002</v>
+      </c>
+      <c r="B39" s="22">
+        <v>3</v>
+      </c>
+      <c r="C39" s="22">
+        <v>2</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="F39" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="G39" s="26"/>
+      <c r="H39">
+        <v>50</v>
+      </c>
+      <c r="I39">
+        <v>-1</v>
+      </c>
+      <c r="Z39" s="26"/>
+      <c r="AA39">
+        <v>1</v>
+      </c>
+      <c r="AK39" s="22" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B30:D30 B4:D17 B19:D28 H18:AJ18 H34:AJ34 B32:D33 H29:AJ31 F32:AJ33 F19:AJ28 F4:AJ17 F30:G30 B35:D36 E4:E36 B38:AJ38 F35:AJ36">
-    <cfRule type="containsBlanks" dxfId="8" priority="15">
+  <conditionalFormatting sqref="B30:D30 B4:D17 B19:D28 I18:AK18 I34:AK34 B32:D33 I29:AK31 F32:AK33 F19:AK28 F4:AK17 F30:H30 B35:D36 E4:E36 B38:AK38 F35:AK36 G4:G39">
+    <cfRule type="containsBlanks" dxfId="11" priority="17">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29:D29 G29">
-    <cfRule type="containsBlanks" dxfId="7" priority="9">
+  <conditionalFormatting sqref="B29:D29 H29">
+    <cfRule type="containsBlanks" dxfId="10" priority="11">
       <formula>LEN(TRIM(B29))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F29">
-    <cfRule type="containsBlanks" dxfId="6" priority="8">
+  <conditionalFormatting sqref="F29:G29">
+    <cfRule type="containsBlanks" dxfId="9" priority="10">
       <formula>LEN(TRIM(F29))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B18:D18 G18">
-    <cfRule type="containsBlanks" dxfId="5" priority="7">
+  <conditionalFormatting sqref="B18:D18 H18">
+    <cfRule type="containsBlanks" dxfId="8" priority="9">
       <formula>LEN(TRIM(B18))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F18">
-    <cfRule type="containsBlanks" dxfId="4" priority="6">
+  <conditionalFormatting sqref="F18:G18">
+    <cfRule type="containsBlanks" dxfId="7" priority="8">
       <formula>LEN(TRIM(F18))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B34:D34 G34">
-    <cfRule type="containsBlanks" dxfId="3" priority="5">
+  <conditionalFormatting sqref="B34:D34 H34">
+    <cfRule type="containsBlanks" dxfId="6" priority="7">
       <formula>LEN(TRIM(B34))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F34">
-    <cfRule type="containsBlanks" dxfId="2" priority="4">
+  <conditionalFormatting sqref="F34:G34">
+    <cfRule type="containsBlanks" dxfId="5" priority="6">
       <formula>LEN(TRIM(F34))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B31:D31 F31:G31">
-    <cfRule type="containsBlanks" dxfId="1" priority="3">
+  <conditionalFormatting sqref="B31:D31 F31:H31">
+    <cfRule type="containsBlanks" dxfId="4" priority="5">
       <formula>LEN(TRIM(B31))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B37:AJ37">
+  <conditionalFormatting sqref="B37:AK37">
+    <cfRule type="containsBlanks" dxfId="3" priority="3">
+      <formula>LEN(TRIM(B37))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39:H39 J39:AK39">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(B39))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I39">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B37))=0</formula>
+      <formula>LEN(TRIM(I39))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>